<commit_message>
DOSINZAGE2-693: Updated maximum cardinality of Performer
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6EE7B8-B2DA-C846-9D80-606698EED84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CDA678-9C46-AD40-A6F6-B3396C47A3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="29080" windowHeight="16400" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19100" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
   <sheets>
     <sheet name="Beeld en verslag tijdlijn raadp" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="277">
   <si>
     <t>Naam</t>
   </si>
@@ -873,6 +873,9 @@
   </si>
   <si>
     <t>Uitgevende instantie van het Accession Number.</t>
+  </si>
+  <si>
+    <t>0 … *</t>
   </si>
 </sst>
 </file>
@@ -1355,12 +1358,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1421,6 +1418,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="25" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1828,60 +1831,55 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="40" t="s">
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="62" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="45"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1889,6 +1887,11 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1902,15 +1905,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="62" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="56" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="38" customWidth="1"/>
-    <col min="3" max="4" width="11" style="63" customWidth="1"/>
+    <col min="3" max="4" width="11" style="57" customWidth="1"/>
     <col min="5" max="5" width="11" style="38" customWidth="1"/>
     <col min="6" max="6" width="105.6640625" style="38" customWidth="1"/>
     <col min="7" max="7" width="44" style="38" bestFit="1" customWidth="1"/>
@@ -1919,7 +1922,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
@@ -1957,7 +1960,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="41" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="32" t="s">
@@ -1981,7 +1984,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="42" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -2008,7 +2011,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="43" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="32" t="s">
@@ -2040,7 +2043,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="44" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -2070,7 +2073,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="43" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -2102,7 +2105,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="32" t="s">
@@ -2134,7 +2137,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -2166,7 +2169,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="46" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="32" t="s">
@@ -2198,7 +2201,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="46" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="32" t="s">
@@ -2232,7 +2235,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="47" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="32" t="s">
@@ -2258,7 +2261,7 @@
       <c r="L11" s="33"/>
     </row>
     <row r="12" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="48" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -2288,7 +2291,7 @@
       <c r="L12" s="33"/>
     </row>
     <row r="13" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="43" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -2318,7 +2321,7 @@
       <c r="L13" s="33"/>
     </row>
     <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="43" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -2350,7 +2353,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="10" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="43" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -2385,7 +2388,7 @@
       <c r="O15" s="35"/>
     </row>
     <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="44" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -2415,7 +2418,7 @@
       <c r="L16" s="33"/>
     </row>
     <row r="17" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="49" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="32" t="s">
@@ -2448,7 +2451,7 @@
       <c r="L17" s="33"/>
     </row>
     <row r="18" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="50" t="s">
         <v>94</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -2468,7 +2471,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="51" t="s">
         <v>273</v>
       </c>
       <c r="B19" s="32" t="s">
@@ -2498,7 +2501,7 @@
       <c r="L19" s="33"/>
     </row>
     <row r="20" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="52" t="s">
         <v>272</v>
       </c>
       <c r="B20" s="32" t="s">
@@ -2528,7 +2531,7 @@
       <c r="L20" s="33"/>
     </row>
     <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="43" t="s">
         <v>103</v>
       </c>
       <c r="B21" s="32" t="s">
@@ -2560,7 +2563,7 @@
       <c r="L21" s="33"/>
     </row>
     <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="43" t="s">
         <v>108</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -2592,7 +2595,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="43" t="s">
         <v>112</v>
       </c>
       <c r="B23" s="32" t="s">
@@ -2624,7 +2627,7 @@
       <c r="L23" s="33"/>
     </row>
     <row r="24" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="50" t="s">
         <v>116</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -2656,7 +2659,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="44" t="s">
         <v>121</v>
       </c>
       <c r="B25" s="32" t="s">
@@ -2684,7 +2687,7 @@
       <c r="L25" s="33"/>
     </row>
     <row r="26" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="51" t="s">
         <v>124</v>
       </c>
       <c r="B26" s="32" t="s">
@@ -2714,7 +2717,7 @@
       <c r="L26" s="33"/>
     </row>
     <row r="27" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="43" t="s">
         <v>129</v>
       </c>
       <c r="B27" s="32" t="s">
@@ -2746,7 +2749,7 @@
       <c r="L27" s="33"/>
     </row>
     <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="44" t="s">
         <v>134</v>
       </c>
       <c r="B28" s="32" t="s">
@@ -2776,7 +2779,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="43" t="s">
         <v>138</v>
       </c>
       <c r="B29" s="32" t="s">
@@ -2808,7 +2811,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="44" t="s">
         <v>142</v>
       </c>
       <c r="B30" s="32" t="s">
@@ -2838,7 +2841,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="43" t="s">
         <v>145</v>
       </c>
       <c r="B31" s="32" t="s">
@@ -2870,7 +2873,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="43" t="s">
         <v>149</v>
       </c>
       <c r="B32" s="32" t="s">
@@ -2902,7 +2905,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="43" t="s">
         <v>153</v>
       </c>
       <c r="B33" s="32" t="s">
@@ -2936,7 +2939,7 @@
       <c r="L33" s="33"/>
     </row>
     <row r="34" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="44" t="s">
         <v>158</v>
       </c>
       <c r="B34" s="32" t="s">
@@ -2946,7 +2949,7 @@
         <v>14</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>33</v>
+        <v>276</v>
       </c>
       <c r="E34" s="33"/>
       <c r="F34" s="32" t="s">
@@ -2961,7 +2964,7 @@
       <c r="L34" s="33"/>
     </row>
     <row r="35" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="51" t="s">
         <v>161</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -2989,7 +2992,7 @@
       <c r="L35" s="12"/>
     </row>
     <row r="36" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="43" t="s">
         <v>164</v>
       </c>
       <c r="B36" s="32" t="s">
@@ -3021,7 +3024,7 @@
       <c r="L36" s="33"/>
     </row>
     <row r="37" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="44" t="s">
         <v>166</v>
       </c>
       <c r="B37" s="32" t="s">
@@ -3051,7 +3054,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="43" t="s">
         <v>168</v>
       </c>
       <c r="B38" s="32" t="s">
@@ -3083,7 +3086,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="50" t="s">
+      <c r="A39" s="44" t="s">
         <v>170</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -3113,7 +3116,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="43" t="s">
         <v>172</v>
       </c>
       <c r="B40" s="32" t="s">
@@ -3145,7 +3148,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="43" t="s">
         <v>174</v>
       </c>
       <c r="B41" s="32" t="s">
@@ -3177,7 +3180,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="43" t="s">
         <v>176</v>
       </c>
       <c r="B42" s="32" t="s">
@@ -3211,7 +3214,7 @@
       <c r="L42" s="33"/>
     </row>
     <row r="43" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="43" t="s">
         <v>178</v>
       </c>
       <c r="B43" s="32" t="s">
@@ -3245,7 +3248,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="53" t="s">
         <v>184</v>
       </c>
       <c r="B44" s="32" t="s">
@@ -3273,7 +3276,7 @@
       <c r="L44" s="33"/>
     </row>
     <row r="45" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="43" t="s">
         <v>186</v>
       </c>
       <c r="B45" s="32" t="s">
@@ -3303,7 +3306,7 @@
       <c r="L45" s="33"/>
     </row>
     <row r="46" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="43" t="s">
         <v>190</v>
       </c>
       <c r="B46" s="32" t="s">
@@ -3333,7 +3336,7 @@
       <c r="L46" s="33"/>
     </row>
     <row r="47" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="50" t="s">
         <v>193</v>
       </c>
       <c r="B47" s="11" t="s">
@@ -3361,7 +3364,7 @@
       <c r="L47" s="12"/>
     </row>
     <row r="48" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="60" t="s">
+      <c r="A48" s="54" t="s">
         <v>241</v>
       </c>
       <c r="B48" s="32" t="s">
@@ -3393,7 +3396,7 @@
       <c r="L48" s="33"/>
     </row>
     <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="59" t="s">
+      <c r="A49" s="53" t="s">
         <v>198</v>
       </c>
       <c r="B49" s="32" t="s">
@@ -3421,7 +3424,7 @@
       <c r="L49" s="33"/>
     </row>
     <row r="50" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="43" t="s">
         <v>200</v>
       </c>
       <c r="B50" s="32" t="s">
@@ -3451,7 +3454,7 @@
       <c r="L50" s="33"/>
     </row>
     <row r="51" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="43" t="s">
         <v>203</v>
       </c>
       <c r="B51" s="32" t="s">
@@ -3481,7 +3484,7 @@
       <c r="L51" s="33"/>
     </row>
     <row r="52" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="50" t="s">
         <v>206</v>
       </c>
       <c r="B52" s="11" t="s">
@@ -3508,35 +3511,35 @@
       </c>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A53" s="61" t="s">
+    <row r="53" spans="1:12" s="51" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A53" s="55" t="s">
         <v>256</v>
       </c>
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="51" t="s">
         <v>258</v>
       </c>
-      <c r="C53" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="57" t="s">
+      <c r="C53" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="51" t="s">
         <v>261</v>
       </c>
-      <c r="F53" s="57" t="s">
+      <c r="F53" s="51" t="s">
         <v>262</v>
       </c>
-      <c r="G53" s="64"/>
-      <c r="H53" s="64"/>
-      <c r="I53" s="65"/>
-      <c r="J53" s="64" t="s">
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="59"/>
+      <c r="J53" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="K53" s="57" t="s">
+      <c r="K53" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="L53" s="65"/>
+      <c r="L53" s="59"/>
     </row>
     <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="60" t="s">
+      <c r="A54" s="54" t="s">
         <v>255</v>
       </c>
       <c r="B54" s="32" t="s">
@@ -3566,7 +3569,7 @@
       <c r="L54" s="33"/>
     </row>
     <row r="55" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="60" t="s">
+      <c r="A55" s="54" t="s">
         <v>274</v>
       </c>
       <c r="B55" s="32" t="s">
@@ -3594,7 +3597,7 @@
       <c r="L55" s="33"/>
     </row>
     <row r="56" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="58" t="s">
+      <c r="A56" s="52" t="s">
         <v>271</v>
       </c>
       <c r="B56" s="32" t="s">
@@ -3624,7 +3627,7 @@
       <c r="L56" s="33"/>
     </row>
     <row r="57" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="43" t="s">
         <v>263</v>
       </c>
       <c r="B57" s="32" t="s">
@@ -3656,7 +3659,7 @@
       <c r="L57" s="33"/>
     </row>
     <row r="58" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="43" t="s">
         <v>264</v>
       </c>
       <c r="B58" s="32" t="s">
@@ -3688,7 +3691,7 @@
       </c>
     </row>
     <row r="59" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="43" t="s">
         <v>112</v>
       </c>
       <c r="B59" s="32" t="s">
@@ -3720,7 +3723,7 @@
       <c r="L59" s="33"/>
     </row>
     <row r="60" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="56" t="s">
+      <c r="A60" s="50" t="s">
         <v>265</v>
       </c>
       <c r="B60" s="32" t="s">
@@ -3752,7 +3755,7 @@
       </c>
     </row>
     <row r="61" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="61" t="s">
+      <c r="A61" s="55" t="s">
         <v>235</v>
       </c>
       <c r="B61" s="32" t="s">
@@ -4748,12 +4751,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4986,20 +4991,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5024,12 +5030,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DOSINZAGE2-684: Finetuned requirements based on internal feedback
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6EE7B8-B2DA-C846-9D80-606698EED84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522F6753-578A-3648-916D-5F33F06D769D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="29080" windowHeight="16400" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
@@ -524,9 +524,6 @@
     <t>bbs-dataelement-187</t>
   </si>
   <si>
-    <t>De zorgverlener die de verrichting heeft uitgevoerd of zal uitvoeren. In de meeste gevallen wordt alleen het specialisme en niet de naam van de zorgverlener doorgegeven.</t>
-  </si>
-  <si>
     <t> 2.1.7.1.Zorgverlener</t>
   </si>
   <si>
@@ -873,13 +870,17 @@
   </si>
   <si>
     <t>Uitgevende instantie van het Accession Number.</t>
+  </si>
+  <si>
+    <t>De zorgverlener die de verrichting heeft uitgevoerd of zal uitvoeren. In de meeste gevallen wordt alleen het specialisme en niet de naam van de zorgverlener doorgegeven.
+Voor Beelduitwisseling wordt hiermee de uitvoerende arts (Performing Physician) bedoeld en NIET de laborant die de beelden maakt (Operator).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1282,7 +1283,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1345,9 +1346,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1355,12 +1353,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1420,6 +1412,27 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="25" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="26">
@@ -1781,7 +1794,7 @@
       <selection activeCell="G1" activeCellId="1" sqref="F1:F1048576 G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="5" width="11" customWidth="1"/>
@@ -1789,7 +1802,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1827,61 +1840,56 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1">
+      <c r="A2" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="40" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="61" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="45"/>
+    <row r="3" spans="1:12" s="2" customFormat="1">
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1889,6 +1897,11 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1902,24 +1915,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="62" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" style="38" customWidth="1"/>
-    <col min="3" max="4" width="11" style="63" customWidth="1"/>
-    <col min="5" max="5" width="11" style="38" customWidth="1"/>
-    <col min="6" max="6" width="105.6640625" style="38" customWidth="1"/>
-    <col min="7" max="7" width="44" style="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="241" width="11" style="38" customWidth="1"/>
-    <col min="242" max="16384" width="8.83203125" style="38"/>
+    <col min="1" max="1" width="26.5" style="55" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="37" customWidth="1"/>
+    <col min="3" max="4" width="11" style="56" customWidth="1"/>
+    <col min="5" max="5" width="11" style="37" customWidth="1"/>
+    <col min="6" max="6" width="105.6640625" style="69" customWidth="1"/>
+    <col min="7" max="7" width="44" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="241" width="11" style="37" customWidth="1"/>
+    <col min="242" max="16384" width="8.83203125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:15" s="10" customFormat="1">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
@@ -1934,7 +1947,7 @@
       <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="31" t="s">
@@ -1956,8 +1969,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:15" s="34" customFormat="1">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="32" t="s">
@@ -1970,7 +1983,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="33"/>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="30" t="s">
         <v>24</v>
       </c>
       <c r="J2" s="32" t="s">
@@ -1980,8 +1993,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:15" s="10" customFormat="1">
+      <c r="A3" s="41" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1994,7 +2007,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="66" t="s">
         <v>29</v>
       </c>
       <c r="J3" s="11" t="s">
@@ -2007,8 +2020,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
+    <row r="4" spans="1:15" s="10" customFormat="1">
+      <c r="A4" s="42" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="32" t="s">
@@ -2023,7 +2036,7 @@
       <c r="E4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>35</v>
       </c>
       <c r="G4" s="34"/>
@@ -2039,8 +2052,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:15" s="10" customFormat="1">
+      <c r="A5" s="43" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -2053,7 +2066,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="33"/>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="30" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="34"/>
@@ -2069,8 +2082,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
+    <row r="6" spans="1:15" s="10" customFormat="1">
+      <c r="A6" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -2085,7 +2098,7 @@
       <c r="E6" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="30" t="s">
         <v>44</v>
       </c>
       <c r="G6" s="34"/>
@@ -2101,8 +2114,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+    <row r="7" spans="1:15" s="10" customFormat="1">
+      <c r="A7" s="42" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="32" t="s">
@@ -2117,7 +2130,7 @@
       <c r="E7" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="30" t="s">
         <v>49</v>
       </c>
       <c r="G7" s="34"/>
@@ -2133,8 +2146,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A8" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -2149,7 +2162,7 @@
       <c r="E8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="66" t="s">
         <v>52</v>
       </c>
       <c r="G8" s="11" t="s">
@@ -2165,8 +2178,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52" t="s">
+    <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A9" s="45" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="32" t="s">
@@ -2181,7 +2194,7 @@
       <c r="E9" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="30" t="s">
         <v>57</v>
       </c>
       <c r="G9" s="34"/>
@@ -2197,8 +2210,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
+    <row r="10" spans="1:15" s="10" customFormat="1">
+      <c r="A10" s="45" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="32" t="s">
@@ -2213,7 +2226,7 @@
       <c r="E10" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G10" s="34"/>
@@ -2231,8 +2244,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+    <row r="11" spans="1:15" s="10" customFormat="1">
+      <c r="A11" s="46" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="32" t="s">
@@ -2245,7 +2258,7 @@
         <v>67</v>
       </c>
       <c r="E11" s="33"/>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="30" t="s">
         <v>68</v>
       </c>
       <c r="G11" s="34"/>
@@ -2257,8 +2270,8 @@
       <c r="K11" s="34"/>
       <c r="L11" s="33"/>
     </row>
-    <row r="12" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
+    <row r="12" spans="1:15" s="10" customFormat="1">
+      <c r="A12" s="47" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -2271,7 +2284,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="33"/>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="30" t="s">
         <v>71</v>
       </c>
       <c r="G12" s="34"/>
@@ -2287,8 +2300,8 @@
       </c>
       <c r="L12" s="33"/>
     </row>
-    <row r="13" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="49" t="s">
+    <row r="13" spans="1:15" s="10" customFormat="1">
+      <c r="A13" s="42" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -2303,7 +2316,7 @@
       <c r="E13" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="66" t="s">
         <v>76</v>
       </c>
       <c r="G13" s="34"/>
@@ -2317,8 +2330,8 @@
       </c>
       <c r="L13" s="33"/>
     </row>
-    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+    <row r="14" spans="1:15" s="10" customFormat="1">
+      <c r="A14" s="42" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -2333,7 +2346,7 @@
       <c r="E14" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="66" t="s">
         <v>80</v>
       </c>
       <c r="G14" s="34"/>
@@ -2349,8 +2362,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="10" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A15" s="49" t="s">
+    <row r="15" spans="1:15" s="10" customFormat="1" ht="105">
+      <c r="A15" s="42" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -2366,7 +2379,7 @@
         <v>61</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
@@ -2384,8 +2397,8 @@
       <c r="N15" s="35"/>
       <c r="O15" s="35"/>
     </row>
-    <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="50" t="s">
+    <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1">
+      <c r="A16" s="43" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -2398,8 +2411,8 @@
         <v>33</v>
       </c>
       <c r="E16" s="33"/>
-      <c r="F16" s="36" t="s">
-        <v>249</v>
+      <c r="F16" s="67" t="s">
+        <v>248</v>
       </c>
       <c r="G16" s="34"/>
       <c r="H16" s="33" t="s">
@@ -2414,8 +2427,8 @@
       </c>
       <c r="L16" s="33"/>
     </row>
-    <row r="17" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="55" t="s">
+    <row r="17" spans="1:12" s="34" customFormat="1">
+      <c r="A17" s="48" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="32" t="s">
@@ -2430,7 +2443,7 @@
       <c r="E17" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="67" t="s">
         <v>90</v>
       </c>
       <c r="H17" s="33" t="s">
@@ -2447,8 +2460,8 @@
       </c>
       <c r="L17" s="33"/>
     </row>
-    <row r="18" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="56" t="s">
+    <row r="18" spans="1:12" s="10" customFormat="1">
+      <c r="A18" s="49" t="s">
         <v>94</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -2463,13 +2476,13 @@
       <c r="E18" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
-        <v>273</v>
+      <c r="F18" s="66" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1">
+      <c r="A19" s="50" t="s">
+        <v>272</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>97</v>
@@ -2481,7 +2494,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="33"/>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="30" t="s">
         <v>98</v>
       </c>
       <c r="G19" s="34"/>
@@ -2497,9 +2510,9 @@
       </c>
       <c r="L19" s="33"/>
     </row>
-    <row r="20" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="58" t="s">
-        <v>272</v>
+    <row r="20" spans="1:12" s="10" customFormat="1">
+      <c r="A20" s="51" t="s">
+        <v>271</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>100</v>
@@ -2511,7 +2524,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="33"/>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="30" t="s">
         <v>101</v>
       </c>
       <c r="G20" s="34"/>
@@ -2527,8 +2540,8 @@
       </c>
       <c r="L20" s="33"/>
     </row>
-    <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49" t="s">
+    <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="42" t="s">
         <v>103</v>
       </c>
       <c r="B21" s="32" t="s">
@@ -2543,7 +2556,7 @@
       <c r="E21" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="30" t="s">
         <v>105</v>
       </c>
       <c r="G21" s="32" t="s">
@@ -2559,8 +2572,8 @@
       </c>
       <c r="L21" s="33"/>
     </row>
-    <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+    <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+      <c r="A22" s="42" t="s">
         <v>108</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -2575,7 +2588,7 @@
       <c r="E22" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="30" t="s">
         <v>110</v>
       </c>
       <c r="G22" s="34"/>
@@ -2591,8 +2604,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="49" t="s">
+    <row r="23" spans="1:12" s="10" customFormat="1">
+      <c r="A23" s="42" t="s">
         <v>112</v>
       </c>
       <c r="B23" s="32" t="s">
@@ -2607,7 +2620,7 @@
       <c r="E23" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="66" t="s">
         <v>114</v>
       </c>
       <c r="G23" s="34"/>
@@ -2623,8 +2636,8 @@
       </c>
       <c r="L23" s="33"/>
     </row>
-    <row r="24" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="56" t="s">
+    <row r="24" spans="1:12" s="10" customFormat="1">
+      <c r="A24" s="49" t="s">
         <v>116</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -2639,7 +2652,7 @@
       <c r="E24" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="66" t="s">
         <v>118</v>
       </c>
       <c r="I24" s="12" t="s">
@@ -2655,8 +2668,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="50" t="s">
+    <row r="25" spans="1:12" s="10" customFormat="1">
+      <c r="A25" s="43" t="s">
         <v>121</v>
       </c>
       <c r="B25" s="32" t="s">
@@ -2669,7 +2682,7 @@
         <v>33</v>
       </c>
       <c r="E25" s="33"/>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="66" t="s">
         <v>123</v>
       </c>
       <c r="G25" s="34"/>
@@ -2683,8 +2696,8 @@
       </c>
       <c r="L25" s="33"/>
     </row>
-    <row r="26" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="57" t="s">
+    <row r="26" spans="1:12" s="10" customFormat="1">
+      <c r="A26" s="50" t="s">
         <v>124</v>
       </c>
       <c r="B26" s="32" t="s">
@@ -2697,7 +2710,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="33"/>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="66" t="s">
         <v>126</v>
       </c>
       <c r="G26" s="34"/>
@@ -2713,8 +2726,8 @@
       </c>
       <c r="L26" s="33"/>
     </row>
-    <row r="27" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+    <row r="27" spans="1:12" s="10" customFormat="1">
+      <c r="A27" s="42" t="s">
         <v>129</v>
       </c>
       <c r="B27" s="32" t="s">
@@ -2729,7 +2742,7 @@
       <c r="E27" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="30" t="s">
         <v>131</v>
       </c>
       <c r="G27" s="32" t="s">
@@ -2745,8 +2758,8 @@
       </c>
       <c r="L27" s="33"/>
     </row>
-    <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="50" t="s">
+    <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A28" s="43" t="s">
         <v>134</v>
       </c>
       <c r="B28" s="32" t="s">
@@ -2759,7 +2772,7 @@
         <v>15</v>
       </c>
       <c r="E28" s="33"/>
-      <c r="F28" s="32" t="s">
+      <c r="F28" s="30" t="s">
         <v>136</v>
       </c>
       <c r="G28" s="34"/>
@@ -2775,8 +2788,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="49" t="s">
+    <row r="29" spans="1:12" s="10" customFormat="1">
+      <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
       <c r="B29" s="32" t="s">
@@ -2791,7 +2804,7 @@
       <c r="E29" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="F29" s="30" t="s">
         <v>140</v>
       </c>
       <c r="G29" s="34"/>
@@ -2807,8 +2820,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="50" t="s">
+    <row r="30" spans="1:12" s="10" customFormat="1">
+      <c r="A30" s="43" t="s">
         <v>142</v>
       </c>
       <c r="B30" s="32" t="s">
@@ -2821,7 +2834,7 @@
         <v>15</v>
       </c>
       <c r="E30" s="33"/>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="30" t="s">
         <v>40</v>
       </c>
       <c r="G30" s="34"/>
@@ -2837,8 +2850,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="49" t="s">
+    <row r="31" spans="1:12" s="10" customFormat="1">
+      <c r="A31" s="42" t="s">
         <v>145</v>
       </c>
       <c r="B31" s="32" t="s">
@@ -2853,7 +2866,7 @@
       <c r="E31" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F31" s="32" t="s">
+      <c r="F31" s="30" t="s">
         <v>147</v>
       </c>
       <c r="G31" s="34"/>
@@ -2869,8 +2882,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="49" t="s">
+    <row r="32" spans="1:12" s="10" customFormat="1">
+      <c r="A32" s="42" t="s">
         <v>149</v>
       </c>
       <c r="B32" s="32" t="s">
@@ -2885,7 +2898,7 @@
       <c r="E32" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="30" t="s">
         <v>151</v>
       </c>
       <c r="G32" s="34"/>
@@ -2901,8 +2914,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="49" t="s">
+    <row r="33" spans="1:12" s="10" customFormat="1">
+      <c r="A33" s="42" t="s">
         <v>153</v>
       </c>
       <c r="B33" s="32" t="s">
@@ -2917,7 +2930,7 @@
       <c r="E33" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="30" t="s">
         <v>155</v>
       </c>
       <c r="G33" s="34"/>
@@ -2935,8 +2948,8 @@
       </c>
       <c r="L33" s="33"/>
     </row>
-    <row r="34" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="50" t="s">
+    <row r="34" spans="1:12" s="34" customFormat="1" ht="45">
+      <c r="A34" s="43" t="s">
         <v>158</v>
       </c>
       <c r="B34" s="32" t="s">
@@ -2949,8 +2962,8 @@
         <v>33</v>
       </c>
       <c r="E34" s="33"/>
-      <c r="F34" s="32" t="s">
-        <v>160</v>
+      <c r="F34" s="30" t="s">
+        <v>275</v>
       </c>
       <c r="J34" s="32" t="s">
         <v>25</v>
@@ -2960,12 +2973,12 @@
       </c>
       <c r="L34" s="33"/>
     </row>
-    <row r="35" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="57" t="s">
+    <row r="35" spans="1:12" s="10" customFormat="1">
+      <c r="A35" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>161</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>162</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>14</v>
@@ -2974,7 +2987,7 @@
         <v>15</v>
       </c>
       <c r="E35" s="12"/>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="66" t="s">
         <v>126</v>
       </c>
       <c r="H35" s="12" t="s">
@@ -2984,16 +2997,16 @@
         <v>25</v>
       </c>
       <c r="K35" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="L35" s="12"/>
+    </row>
+    <row r="36" spans="1:12" s="10" customFormat="1">
+      <c r="A36" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="L35" s="12"/>
-    </row>
-    <row r="36" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="49" t="s">
+      <c r="B36" s="32" t="s">
         <v>164</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>165</v>
       </c>
       <c r="C36" s="32" t="s">
         <v>14</v>
@@ -3004,7 +3017,7 @@
       <c r="E36" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="32" t="s">
+      <c r="F36" s="30" t="s">
         <v>131</v>
       </c>
       <c r="G36" s="32" t="s">
@@ -3020,12 +3033,12 @@
       </c>
       <c r="L36" s="33"/>
     </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="50" t="s">
+    <row r="37" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+      <c r="A37" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" s="32" t="s">
         <v>166</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>167</v>
       </c>
       <c r="C37" s="32" t="s">
         <v>14</v>
@@ -3034,7 +3047,7 @@
         <v>15</v>
       </c>
       <c r="E37" s="33"/>
-      <c r="F37" s="32" t="s">
+      <c r="F37" s="30" t="s">
         <v>136</v>
       </c>
       <c r="G37" s="34"/>
@@ -3050,12 +3063,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="49" t="s">
+    <row r="38" spans="1:12" s="10" customFormat="1">
+      <c r="A38" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" s="32" t="s">
         <v>168</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>169</v>
       </c>
       <c r="C38" s="32" t="s">
         <v>14</v>
@@ -3066,7 +3079,7 @@
       <c r="E38" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="30" t="s">
         <v>140</v>
       </c>
       <c r="G38" s="34"/>
@@ -3082,12 +3095,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="50" t="s">
+    <row r="39" spans="1:12" s="10" customFormat="1">
+      <c r="A39" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" s="32" t="s">
         <v>170</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>171</v>
       </c>
       <c r="C39" s="32" t="s">
         <v>14</v>
@@ -3096,7 +3109,7 @@
         <v>15</v>
       </c>
       <c r="E39" s="33"/>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="30" t="s">
         <v>40</v>
       </c>
       <c r="G39" s="34"/>
@@ -3112,12 +3125,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="49" t="s">
+    <row r="40" spans="1:12" s="10" customFormat="1">
+      <c r="A40" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" s="32" t="s">
         <v>172</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>173</v>
       </c>
       <c r="C40" s="32" t="s">
         <v>14</v>
@@ -3128,7 +3141,7 @@
       <c r="E40" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="30" t="s">
         <v>147</v>
       </c>
       <c r="G40" s="34"/>
@@ -3144,12 +3157,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="49" t="s">
+    <row r="41" spans="1:12" s="10" customFormat="1">
+      <c r="A41" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="32" t="s">
         <v>174</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>175</v>
       </c>
       <c r="C41" s="32" t="s">
         <v>14</v>
@@ -3160,7 +3173,7 @@
       <c r="E41" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F41" s="32" t="s">
+      <c r="F41" s="30" t="s">
         <v>151</v>
       </c>
       <c r="G41" s="34"/>
@@ -3176,12 +3189,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="49" t="s">
+    <row r="42" spans="1:12" s="10" customFormat="1">
+      <c r="A42" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="32" t="s">
         <v>176</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>177</v>
       </c>
       <c r="C42" s="32" t="s">
         <v>14</v>
@@ -3192,7 +3205,7 @@
       <c r="E42" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F42" s="32" t="s">
+      <c r="F42" s="30" t="s">
         <v>155</v>
       </c>
       <c r="G42" s="34"/>
@@ -3210,29 +3223,29 @@
       </c>
       <c r="L42" s="33"/>
     </row>
-    <row r="43" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="49" t="s">
+    <row r="43" spans="1:12" s="10" customFormat="1">
+      <c r="A43" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="B43" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="C43" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="32" t="s">
         <v>179</v>
-      </c>
-      <c r="C43" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>180</v>
       </c>
       <c r="E43" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F43" s="32" t="s">
-        <v>181</v>
+      <c r="F43" s="30" t="s">
+        <v>180</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
       <c r="I43" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J43" s="32" t="s">
         <v>19</v>
@@ -3241,25 +3254,25 @@
         <v>133</v>
       </c>
       <c r="L43" s="33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="10" customFormat="1">
+      <c r="A44" s="52" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="59" t="s">
+      <c r="B44" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="B44" s="32" t="s">
-        <v>185</v>
-      </c>
       <c r="C44" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="36" t="s">
         <v>33</v>
       </c>
       <c r="E44" s="33"/>
-      <c r="F44" s="32" t="s">
-        <v>247</v>
+      <c r="F44" s="30" t="s">
+        <v>246</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
@@ -3272,12 +3285,12 @@
       </c>
       <c r="L44" s="33"/>
     </row>
-    <row r="45" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="49" t="s">
+    <row r="45" spans="1:12" s="10" customFormat="1">
+      <c r="A45" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="B45" s="32" t="s">
         <v>186</v>
-      </c>
-      <c r="B45" s="32" t="s">
-        <v>187</v>
       </c>
       <c r="C45" s="32" t="s">
         <v>14</v>
@@ -3288,8 +3301,8 @@
       <c r="E45" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="32" t="s">
-        <v>246</v>
+      <c r="F45" s="30" t="s">
+        <v>245</v>
       </c>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
@@ -3298,16 +3311,16 @@
         <v>19</v>
       </c>
       <c r="K45" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="L45" s="33"/>
+    </row>
+    <row r="46" spans="1:12" s="10" customFormat="1">
+      <c r="A46" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="L45" s="33"/>
-    </row>
-    <row r="46" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="49" t="s">
+      <c r="B46" s="32" t="s">
         <v>190</v>
-      </c>
-      <c r="B46" s="32" t="s">
-        <v>191</v>
       </c>
       <c r="C46" s="32" t="s">
         <v>14</v>
@@ -3318,8 +3331,8 @@
       <c r="E46" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="32" t="s">
-        <v>192</v>
+      <c r="F46" s="30" t="s">
+        <v>191</v>
       </c>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
@@ -3328,76 +3341,76 @@
         <v>19</v>
       </c>
       <c r="K46" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L46" s="33"/>
     </row>
-    <row r="47" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="56" t="s">
+    <row r="47" spans="1:12" s="10" customFormat="1">
+      <c r="A47" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="B47" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="C47" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>194</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>195</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F47" s="11" t="s">
-        <v>197</v>
+      <c r="F47" s="66" t="s">
+        <v>196</v>
       </c>
       <c r="I47" s="12"/>
       <c r="J47" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="60" t="s">
+    <row r="48" spans="1:12" s="10" customFormat="1">
+      <c r="A48" s="53" t="s">
+        <v>240</v>
+      </c>
+      <c r="B48" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="C48" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="32" t="s">
         <v>242</v>
-      </c>
-      <c r="C48" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="32" t="s">
-        <v>243</v>
       </c>
       <c r="E48" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F48" s="32" t="s">
-        <v>253</v>
+      <c r="F48" s="30" t="s">
+        <v>252</v>
       </c>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
       <c r="I48" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J48" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K48" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L48" s="33"/>
     </row>
-    <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="59" t="s">
+    <row r="49" spans="1:12" s="10" customFormat="1">
+      <c r="A49" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="B49" s="32" t="s">
         <v>198</v>
-      </c>
-      <c r="B49" s="32" t="s">
-        <v>199</v>
       </c>
       <c r="C49" s="32" t="s">
         <v>14</v>
@@ -3406,8 +3419,8 @@
         <v>33</v>
       </c>
       <c r="E49" s="33"/>
-      <c r="F49" s="32" t="s">
-        <v>248</v>
+      <c r="F49" s="30" t="s">
+        <v>247</v>
       </c>
       <c r="G49" s="34"/>
       <c r="H49" s="34"/>
@@ -3420,12 +3433,12 @@
       </c>
       <c r="L49" s="33"/>
     </row>
-    <row r="50" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="49" t="s">
+    <row r="50" spans="1:12" s="10" customFormat="1">
+      <c r="A50" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B50" s="32" t="s">
         <v>200</v>
-      </c>
-      <c r="B50" s="32" t="s">
-        <v>201</v>
       </c>
       <c r="C50" s="32" t="s">
         <v>14</v>
@@ -3436,8 +3449,8 @@
       <c r="E50" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F50" s="32" t="s">
-        <v>245</v>
+      <c r="F50" s="30" t="s">
+        <v>244</v>
       </c>
       <c r="G50" s="34"/>
       <c r="H50" s="34"/>
@@ -3446,16 +3459,16 @@
         <v>19</v>
       </c>
       <c r="K50" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="L50" s="33"/>
+    </row>
+    <row r="51" spans="1:12" s="10" customFormat="1">
+      <c r="A51" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="L50" s="33"/>
-    </row>
-    <row r="51" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="49" t="s">
+      <c r="B51" s="32" t="s">
         <v>203</v>
-      </c>
-      <c r="B51" s="32" t="s">
-        <v>204</v>
       </c>
       <c r="C51" s="32" t="s">
         <v>14</v>
@@ -3466,8 +3479,8 @@
       <c r="E51" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F51" s="32" t="s">
-        <v>205</v>
+      <c r="F51" s="30" t="s">
+        <v>204</v>
       </c>
       <c r="G51" s="34"/>
       <c r="H51" s="34"/>
@@ -3476,83 +3489,83 @@
         <v>19</v>
       </c>
       <c r="K51" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L51" s="33"/>
     </row>
-    <row r="52" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="56" t="s">
+    <row r="52" spans="1:12" s="10" customFormat="1">
+      <c r="A52" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>207</v>
-      </c>
       <c r="C52" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F52" s="11" t="s">
-        <v>244</v>
+      <c r="F52" s="66" t="s">
+        <v>243</v>
       </c>
       <c r="I52" s="12"/>
       <c r="J52" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K52" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A53" s="61" t="s">
-        <v>256</v>
-      </c>
-      <c r="B53" s="57" t="s">
+    <row r="53" spans="1:12" s="50" customFormat="1" ht="15">
+      <c r="A53" s="54" t="s">
+        <v>255</v>
+      </c>
+      <c r="B53" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="C53" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="F53" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="58"/>
+      <c r="J53" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="K53" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" s="58"/>
+    </row>
+    <row r="54" spans="1:12" s="10" customFormat="1">
+      <c r="A54" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="B54" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="32" t="s">
         <v>258</v>
-      </c>
-      <c r="C53" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F53" s="57" t="s">
-        <v>262</v>
-      </c>
-      <c r="G53" s="64"/>
-      <c r="H53" s="64"/>
-      <c r="I53" s="65"/>
-      <c r="J53" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="K53" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="L53" s="65"/>
-    </row>
-    <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="60" t="s">
-        <v>255</v>
-      </c>
-      <c r="B54" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="C54" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="32" t="s">
-        <v>259</v>
       </c>
       <c r="E54" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F54" s="32" t="s">
-        <v>237</v>
+      <c r="F54" s="30" t="s">
+        <v>236</v>
       </c>
       <c r="G54" s="34"/>
       <c r="H54" s="34"/>
@@ -3561,26 +3574,26 @@
         <v>19</v>
       </c>
       <c r="K54" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L54" s="33"/>
     </row>
-    <row r="55" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="60" t="s">
+    <row r="55" spans="1:12" s="10" customFormat="1">
+      <c r="A55" s="53" t="s">
+        <v>273</v>
+      </c>
+      <c r="B55" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E55" s="33"/>
+      <c r="F55" s="30" t="s">
         <v>274</v>
-      </c>
-      <c r="B55" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="C55" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="32" t="s">
-        <v>259</v>
-      </c>
-      <c r="E55" s="33"/>
-      <c r="F55" s="32" t="s">
-        <v>275</v>
       </c>
       <c r="G55" s="34"/>
       <c r="H55" s="34"/>
@@ -3589,25 +3602,25 @@
         <v>19</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L55" s="33"/>
     </row>
-    <row r="56" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="58" t="s">
-        <v>271</v>
+    <row r="56" spans="1:12" s="10" customFormat="1">
+      <c r="A56" s="51" t="s">
+        <v>270</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C56" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E56" s="33"/>
-      <c r="F56" s="32" t="s">
+      <c r="F56" s="30" t="s">
         <v>101</v>
       </c>
       <c r="G56" s="34"/>
@@ -3623,23 +3636,23 @@
       </c>
       <c r="L56" s="33"/>
     </row>
-    <row r="57" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="49" t="s">
-        <v>263</v>
+    <row r="57" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
+      <c r="A57" s="42" t="s">
+        <v>262</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C57" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E57" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F57" s="32" t="s">
+      <c r="F57" s="30" t="s">
         <v>105</v>
       </c>
       <c r="G57" s="32" t="s">
@@ -3655,12 +3668,12 @@
       </c>
       <c r="L57" s="33"/>
     </row>
-    <row r="58" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="49" t="s">
-        <v>264</v>
+    <row r="58" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+      <c r="A58" s="42" t="s">
+        <v>263</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C58" s="32" t="s">
         <v>14</v>
@@ -3671,7 +3684,7 @@
       <c r="E58" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F58" s="32" t="s">
+      <c r="F58" s="30" t="s">
         <v>110</v>
       </c>
       <c r="G58" s="34"/>
@@ -3687,12 +3700,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="49" t="s">
+    <row r="59" spans="1:12" s="10" customFormat="1">
+      <c r="A59" s="42" t="s">
         <v>112</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C59" s="32" t="s">
         <v>14</v>
@@ -3703,7 +3716,7 @@
       <c r="E59" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="66" t="s">
         <v>114</v>
       </c>
       <c r="G59" s="34"/>
@@ -3719,12 +3732,12 @@
       </c>
       <c r="L59" s="33"/>
     </row>
-    <row r="60" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="56" t="s">
-        <v>265</v>
+    <row r="60" spans="1:12" s="10" customFormat="1">
+      <c r="A60" s="49" t="s">
+        <v>264</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>14</v>
@@ -3735,7 +3748,7 @@
       <c r="E60" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F60" s="11" t="s">
+      <c r="F60" s="66" t="s">
         <v>118</v>
       </c>
       <c r="I60" s="12" t="s">
@@ -3751,12 +3764,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="61" t="s">
-        <v>235</v>
+    <row r="61" spans="1:12" s="10" customFormat="1">
+      <c r="A61" s="54" t="s">
+        <v>234</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C61" s="32" t="s">
         <v>14</v>
@@ -3767,8 +3780,8 @@
       <c r="E61" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="32" t="s">
-        <v>236</v>
+      <c r="F61" s="30" t="s">
+        <v>235</v>
       </c>
       <c r="G61" s="34"/>
       <c r="H61" s="34"/>
@@ -3928,13 +3941,13 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3957,7 +3970,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -3972,7 +3985,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -4005,12 +4018,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="2" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>14</v>
@@ -4022,23 +4035,23 @@
         <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H3" s="28"/>
       <c r="J3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="2" customFormat="1">
       <c r="A4" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
@@ -4050,14 +4063,14 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H4" s="27"/>
       <c r="J4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L4" s="3"/>
     </row>
@@ -4082,7 +4095,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="17" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -4091,7 +4104,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="2" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4129,9 +4142,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="2" customFormat="1">
       <c r="A2" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>23</v>
@@ -4153,7 +4166,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="2" customFormat="1">
       <c r="A3" s="24" t="s">
         <v>27</v>
       </c>
@@ -4180,7 +4193,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="2" customFormat="1">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -4209,7 +4222,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="2" customFormat="1">
       <c r="A5" s="16" t="s">
         <v>38</v>
       </c>
@@ -4236,7 +4249,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="2" customFormat="1">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -4253,7 +4266,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>19</v>
@@ -4265,7 +4278,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="2" customFormat="1">
       <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
@@ -4294,7 +4307,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="23" t="s">
         <v>51</v>
       </c>
@@ -4326,7 +4339,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="23" t="s">
         <v>53</v>
       </c>
@@ -4343,7 +4356,7 @@
         <v>56</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>19</v>
@@ -4355,7 +4368,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="2" customFormat="1">
       <c r="A10" s="23" t="s">
         <v>59</v>
       </c>
@@ -4372,7 +4385,7 @@
         <v>61</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>63</v>
@@ -4387,7 +4400,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="2" customFormat="1">
       <c r="A11" s="26" t="s">
         <v>65</v>
       </c>
@@ -4413,22 +4426,22 @@
       <c r="K11" s="20"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="2" customFormat="1">
       <c r="A12" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -4441,12 +4454,12 @@
       </c>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="2" customFormat="1">
       <c r="A13" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>14</v>
@@ -4458,7 +4471,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -4467,16 +4480,16 @@
         <v>19</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="2" customFormat="1">
       <c r="A14" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>14</v>
@@ -4488,7 +4501,7 @@
         <v>56</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -4497,56 +4510,56 @@
         <v>19</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="2" customFormat="1">
       <c r="A15" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="2" customFormat="1">
       <c r="A16" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="39" t="s">
-        <v>238</v>
+      <c r="F16" s="38" t="s">
+        <v>237</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -4555,22 +4568,22 @@
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="2" customFormat="1">
       <c r="A17" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -4583,12 +4596,12 @@
       </c>
       <c r="L17" s="21"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="2" customFormat="1">
       <c r="A18" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>14</v>
@@ -4600,7 +4613,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -4609,16 +4622,16 @@
         <v>19</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L18" s="21"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" s="2" customFormat="1">
       <c r="A19" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>14</v>
@@ -4630,7 +4643,7 @@
         <v>56</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -4639,46 +4652,46 @@
         <v>19</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L19" s="21"/>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="2" customFormat="1">
       <c r="A20" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" s="4" customFormat="1" ht="14">
       <c r="A21" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>14</v>
@@ -4687,18 +4700,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="9"/>
-      <c r="F21" s="39" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F21" s="38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="29" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -4748,12 +4761,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4986,20 +5001,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5024,12 +5040,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DOSINZAGE2-681: Added Initials to dataset (for Patient, Requester and Performer)
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D605F28-540E-A64C-BC82-6179099E6EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7009909E-2544-804D-8A70-C750E0C3A2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="29080" windowHeight="16400" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
+    <workbookView xWindow="29560" yWindow="660" windowWidth="34160" windowHeight="27980" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
   <sheets>
     <sheet name="Beeld en verslag tijdlijn raadp" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name=" Beeld &amp;Verslag beschikbaar" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Beeld en verslag tijdlijn besch'!$A$1:$N$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Beeld en verslag tijdlijn besch'!$A$1:$N$55</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="286">
   <si>
     <t>Naam</t>
   </si>
@@ -158,9 +158,6 @@
     <t>zib2020bbr-dataelementen-287</t>
   </si>
   <si>
-    <t> 1.1.2. Geslachtsnaam</t>
-  </si>
-  <si>
     <t>bbs-dataelement-138</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>zib2020bbr-dataelementen-291</t>
   </si>
   <si>
-    <t>1.1.2.1. Voorvoegsels</t>
-  </si>
-  <si>
     <t>bbs-dataelement-139</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>zib2020bbr-dataelementen-292</t>
   </si>
   <si>
-    <t>1.1.2.2. Achternaam</t>
-  </si>
-  <si>
     <t>bbs-dataelement-140</t>
   </si>
   <si>
@@ -470,18 +461,12 @@
     <t>zib2020bbr-dataelementen-496</t>
   </si>
   <si>
-    <t> 2.1.6.1.2.2 Geslachtsnaam</t>
-  </si>
-  <si>
     <t>bbs-dataelement-430</t>
   </si>
   <si>
     <t>zib2020bbr-dataelementen-500</t>
   </si>
   <si>
-    <t> 2.1.6.1.2.2.1. Voorvoegsels</t>
-  </si>
-  <si>
     <t>bbs-dataelement-431</t>
   </si>
   <si>
@@ -491,9 +476,6 @@
     <t>zib2020bbr-dataelementen-501</t>
   </si>
   <si>
-    <t> 2.1.6.1.2.2.1. Achternaam</t>
-  </si>
-  <si>
     <t>bbs-dataelement-432</t>
   </si>
   <si>
@@ -551,19 +533,10 @@
     <t>bbs-dataelement-386</t>
   </si>
   <si>
-    <t> 2.1.7.1.2.2 Geslachtsnaam</t>
-  </si>
-  <si>
     <t>bbs-dataelement-390</t>
   </si>
   <si>
-    <t> 2.1.7.1.2.2.1Voorvoegsels</t>
-  </si>
-  <si>
     <t>bbs-dataelement-391</t>
-  </si>
-  <si>
-    <t> 2.1.7.1.2.2.1Achternaam</t>
   </si>
   <si>
     <t>bbs-dataelement-392</t>
@@ -773,9 +746,6 @@
     <t>bbs-medmij-dataelement-5</t>
   </si>
   <si>
-    <t>1..*</t>
-  </si>
-  <si>
     <t>De titel van het verslag.</t>
   </si>
   <si>
@@ -877,13 +847,70 @@
   </si>
   <si>
     <t>0 … *</t>
+  </si>
+  <si>
+    <t> 1.1.3. Geslachtsnaam</t>
+  </si>
+  <si>
+    <t>1.1.3.1. Voorvoegsels</t>
+  </si>
+  <si>
+    <t>1.1.3.2. Achternaam</t>
+  </si>
+  <si>
+    <t>1.1.2. Initialen</t>
+  </si>
+  <si>
+    <t>bbs-dataelement-135</t>
+  </si>
+  <si>
+    <t>Initialen van de persoon.</t>
+  </si>
+  <si>
+    <t>zib2020bbr-dataelementen-288</t>
+  </si>
+  <si>
+    <t> 2.1.6.1.2.3.1. Voorvoegsels</t>
+  </si>
+  <si>
+    <t> 2.1.6.1.2.3.1. Achternaam</t>
+  </si>
+  <si>
+    <t> 2.1.6.1.2.3. Geslachtsnaam</t>
+  </si>
+  <si>
+    <t>bbs-dataelement-427</t>
+  </si>
+  <si>
+    <t>zib2020bbr-dataelementen-497</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.1.7.1.2.2. Initialen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.1.6.1.2.2. Initialen</t>
+  </si>
+  <si>
+    <t> 2.1.7.1.2.3. Geslachtsnaam</t>
+  </si>
+  <si>
+    <t> 2.1.7.1.2.3.1. Voorvoegsels</t>
+  </si>
+  <si>
+    <t> 2.1.7.1.2.3.2. Achternaam</t>
+  </si>
+  <si>
+    <t>bbs-dataelement-387</t>
+  </si>
+  <si>
+    <t>1...*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1286,7 +1313,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1433,10 +1460,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1797,7 +1831,7 @@
       <selection activeCell="G1" activeCellId="1" sqref="F1:F1048576 G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="5" width="11" customWidth="1"/>
@@ -1805,7 +1839,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1843,7 +1877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>12</v>
       </c>
@@ -1856,7 +1890,7 @@
       <c r="D2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="66" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="64" t="s">
@@ -1865,39 +1899,34 @@
       <c r="G2" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
       <c r="J2" s="64" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="68" t="s">
+      <c r="L2" s="66" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="65"/>
       <c r="B3" s="65"/>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
-      <c r="E3" s="69"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="65"/>
       <c r="G3" s="65"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
       <c r="J3" s="65"/>
       <c r="K3" s="65"/>
-      <c r="L3" s="69"/>
+      <c r="L3" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1905,6 +1934,11 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1916,13 +1950,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" style="55" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="37" customWidth="1"/>
@@ -1934,7 +1968,7 @@
     <col min="242" max="16384" width="8.83203125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1">
+    <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +2006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="34" customFormat="1">
+    <row r="2" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
@@ -1996,7 +2030,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="10" customFormat="1">
+    <row r="3" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>27</v>
       </c>
@@ -2023,7 +2057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1">
+    <row r="4" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>31</v>
       </c>
@@ -2055,86 +2089,86 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1">
-      <c r="A5" s="43" t="s">
-        <v>38</v>
+    <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="53" t="s">
+        <v>270</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>39</v>
+        <v>271</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="33"/>
+        <v>33</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>34</v>
+      </c>
       <c r="F5" s="30" t="s">
-        <v>40</v>
+        <v>272</v>
       </c>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
       <c r="I5" s="34"/>
       <c r="J5" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K5" s="32" t="s">
         <v>36</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="10" customFormat="1">
-      <c r="A6" s="42" t="s">
-        <v>42</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="43" t="s">
+        <v>267</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>34</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E6" s="33"/>
       <c r="F6" s="30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
       <c r="J6" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K6" s="32" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="10" customFormat="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
-        <v>47</v>
+        <v>268</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
@@ -2143,100 +2177,98 @@
         <v>19</v>
       </c>
       <c r="K7" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="C8" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="45" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A8" s="44" t="s">
+      <c r="B10" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="60" t="s">
+      <c r="C10" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="E10" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="F10" s="30" t="s">
         <v>54</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="10" customFormat="1">
-      <c r="A10" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>62</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="33" t="s">
-        <v>63</v>
-      </c>
+      <c r="I10" s="34"/>
       <c r="J10" s="32" t="s">
         <v>19</v>
       </c>
@@ -2244,71 +2276,75 @@
         <v>20</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="10" customFormat="1">
-      <c r="A11" s="46" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="45" t="s">
+        <v>56</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="33"/>
+        <v>33</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>58</v>
+      </c>
       <c r="F11" s="30" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="I11" s="33" t="s">
+        <v>60</v>
+      </c>
       <c r="J11" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="33"/>
-    </row>
-    <row r="12" spans="1:15" s="10" customFormat="1">
-      <c r="A12" s="47" t="s">
-        <v>69</v>
+        <v>19</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>62</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="30" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G12" s="34"/>
-      <c r="H12" s="33" t="s">
-        <v>72</v>
-      </c>
+      <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="32" t="s">
-        <v>73</v>
-      </c>
+      <c r="K12" s="34"/>
       <c r="L12" s="33"/>
     </row>
-    <row r="13" spans="1:15" s="10" customFormat="1">
-      <c r="A13" s="42" t="s">
-        <v>74</v>
+    <row r="13" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="47" t="s">
+        <v>66</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>14</v>
@@ -2316,41 +2352,41 @@
       <c r="D13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>76</v>
+      <c r="E13" s="33"/>
+      <c r="F13" s="30" t="s">
+        <v>68</v>
       </c>
       <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="33" t="s">
+        <v>69</v>
+      </c>
       <c r="I13" s="34"/>
       <c r="J13" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K13" s="32" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="L13" s="33"/>
     </row>
-    <row r="14" spans="1:15" s="10" customFormat="1">
+    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F14" s="60" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
@@ -2359,166 +2395,166 @@
         <v>19</v>
       </c>
       <c r="K14" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="33"/>
+    </row>
+    <row r="15" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="60" t="s">
         <v>77</v>
-      </c>
-      <c r="L14" s="33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="10" customFormat="1" ht="105">
-      <c r="A15" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>231</v>
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
-      <c r="I15" s="33" t="s">
+      <c r="I15" s="34"/>
+      <c r="J15" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L15" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="10" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A16" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" s="33"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+    </row>
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="61" t="s">
+        <v>238</v>
+      </c>
+      <c r="G17" s="34"/>
+      <c r="H17" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="L15" s="33"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-    </row>
-    <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1">
-      <c r="A16" s="43" t="s">
+      <c r="I17" s="34"/>
+      <c r="J17" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L17" s="33"/>
+    </row>
+    <row r="18" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B18" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="61" t="s">
-        <v>248</v>
-      </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="33" t="s">
+      <c r="C18" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="34"/>
-      <c r="J16" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="L16" s="33"/>
-    </row>
-    <row r="17" spans="1:12" s="34" customFormat="1">
-      <c r="A17" s="48" t="s">
+      <c r="H18" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="I18" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="61" t="s">
+      <c r="J18" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="B19" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J17" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="32" t="s">
+      <c r="C19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L17" s="33"/>
-    </row>
-    <row r="18" spans="1:12" s="10" customFormat="1">
-      <c r="A18" s="49" t="s">
+      <c r="E19" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20" s="32" t="s">
         <v>94</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1">
-      <c r="A19" s="50" t="s">
-        <v>272</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="L19" s="33"/>
-    </row>
-    <row r="20" spans="1:12" s="10" customFormat="1">
-      <c r="A20" s="51" t="s">
-        <v>271</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>100</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>14</v>
@@ -2528,27 +2564,27 @@
       </c>
       <c r="E20" s="33"/>
       <c r="F20" s="30" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G20" s="34"/>
       <c r="H20" s="33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I20" s="34"/>
       <c r="J20" s="32" t="s">
         <v>25</v>
       </c>
       <c r="K20" s="32" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="L20" s="33"/>
     </row>
-    <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="42" t="s">
-        <v>103</v>
+    <row r="21" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="51" t="s">
+        <v>261</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>14</v>
@@ -2556,31 +2592,29 @@
       <c r="D21" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="33" t="s">
-        <v>16</v>
-      </c>
+      <c r="E21" s="33"/>
       <c r="F21" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="34"/>
+        <v>98</v>
+      </c>
+      <c r="G21" s="34"/>
+      <c r="H21" s="33" t="s">
+        <v>96</v>
+      </c>
       <c r="I21" s="34"/>
       <c r="J21" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K21" s="32" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="L21" s="33"/>
     </row>
-    <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+    <row r="22" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="42" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>14</v>
@@ -2589,152 +2623,154 @@
         <v>15</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" s="34"/>
+        <v>102</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="H22" s="34"/>
       <c r="I22" s="34"/>
       <c r="J22" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K22" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L22" s="33"/>
+    </row>
+    <row r="23" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="30" t="s">
         <v>107</v>
-      </c>
-      <c r="L22" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="10" customFormat="1">
-      <c r="A23" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="60" t="s">
-        <v>114</v>
       </c>
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="34"/>
+      <c r="J23" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L23" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L24" s="33"/>
+    </row>
+    <row r="25" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="J23" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K23" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="L23" s="33"/>
-    </row>
-    <row r="24" spans="1:12" s="10" customFormat="1">
-      <c r="A24" s="49" t="s">
+      <c r="I25" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="J25" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="L25" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="11" t="s">
+    </row>
+    <row r="26" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="32" t="s">
         <v>33</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="10" customFormat="1">
-      <c r="A25" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="33"/>
-      <c r="F25" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K25" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="L25" s="33"/>
-    </row>
-    <row r="26" spans="1:12" s="10" customFormat="1">
-      <c r="A26" s="50" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>15</v>
       </c>
       <c r="E26" s="33"/>
       <c r="F26" s="60" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G26" s="34"/>
-      <c r="H26" s="33" t="s">
-        <v>127</v>
-      </c>
+      <c r="H26" s="34"/>
       <c r="I26" s="34"/>
       <c r="J26" s="32" t="s">
         <v>25</v>
       </c>
       <c r="K26" s="32" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="L26" s="33"/>
     </row>
-    <row r="27" spans="1:12" s="10" customFormat="1">
-      <c r="A27" s="42" t="s">
-        <v>129</v>
+    <row r="27" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="50" t="s">
+        <v>121</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C27" s="32" t="s">
         <v>14</v>
@@ -2742,31 +2778,29 @@
       <c r="D27" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="H27" s="34"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="34"/>
+      <c r="H27" s="33" t="s">
+        <v>124</v>
+      </c>
       <c r="I27" s="34"/>
       <c r="J27" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K27" s="32" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="L27" s="33"/>
     </row>
-    <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A28" s="43" t="s">
-        <v>134</v>
+    <row r="28" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="42" t="s">
+        <v>126</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>14</v>
@@ -2774,91 +2808,93 @@
       <c r="D28" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="33"/>
+      <c r="E28" s="33" t="s">
+        <v>16</v>
+      </c>
       <c r="F28" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="G28" s="34"/>
+        <v>128</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>129</v>
+      </c>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
       <c r="J28" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K28" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="L28" s="33"/>
+    </row>
+    <row r="29" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="33"/>
+      <c r="F29" s="30" t="s">
         <v>133</v>
-      </c>
-      <c r="L28" s="33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="10" customFormat="1">
-      <c r="A29" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>140</v>
       </c>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K29" s="32" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="L29" s="33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="10" customFormat="1">
-      <c r="A30" s="43" t="s">
-        <v>142</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="42" t="s">
+        <v>135</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C30" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="33"/>
+        <v>33</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>34</v>
+      </c>
       <c r="F30" s="30" t="s">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K30" s="32" t="s">
         <v>36</v>
       </c>
       <c r="L30" s="33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="10" customFormat="1">
-      <c r="A31" s="42" t="s">
-        <v>145</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="53" t="s">
+        <v>280</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>146</v>
+        <v>277</v>
       </c>
       <c r="C31" s="32" t="s">
         <v>14</v>
@@ -2870,7 +2906,7 @@
         <v>34</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>147</v>
+        <v>272</v>
       </c>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
@@ -2879,18 +2915,18 @@
         <v>19</v>
       </c>
       <c r="K31" s="32" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L31" s="33" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="10" customFormat="1">
-      <c r="A32" s="42" t="s">
-        <v>149</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="43" t="s">
+        <v>276</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C32" s="32" t="s">
         <v>14</v>
@@ -2898,212 +2934,212 @@
       <c r="D32" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="33" t="s">
-        <v>34</v>
-      </c>
+      <c r="E32" s="33"/>
       <c r="F32" s="30" t="s">
-        <v>151</v>
+        <v>39</v>
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
       <c r="J32" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K32" s="32" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L32" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="L34" s="33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G35" s="34"/>
+      <c r="H35" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J35" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="L35" s="33"/>
+    </row>
+    <row r="36" spans="1:12" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A36" s="43" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" s="10" customFormat="1">
-      <c r="A33" s="42" t="s">
+      <c r="B36" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="C36" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="E36" s="33"/>
+      <c r="F36" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="J36" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L36" s="33"/>
+    </row>
+    <row r="37" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="50" t="s">
         <v>154</v>
       </c>
-      <c r="C33" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="32" t="s">
+      <c r="B37" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="33" t="s">
+      <c r="E37" s="12"/>
+      <c r="F37" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="I33" s="33" t="s">
+      <c r="L37" s="12"/>
+    </row>
+    <row r="38" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="J33" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="L33" s="33"/>
-    </row>
-    <row r="34" spans="1:12" s="34" customFormat="1" ht="45">
-      <c r="A34" s="43" t="s">
+      <c r="B38" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="B34" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="C34" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="J34" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K34" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="L34" s="33"/>
-    </row>
-    <row r="35" spans="1:12" s="10" customFormat="1">
-      <c r="A35" s="50" t="s">
-        <v>160</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="11" t="s">
+      <c r="C38" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="60" t="s">
-        <v>126</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="L35" s="12"/>
-    </row>
-    <row r="36" spans="1:12" s="10" customFormat="1">
-      <c r="A36" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="33" t="s">
+      <c r="E38" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="G36" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K36" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="L36" s="33"/>
-    </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
-      <c r="A37" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="33"/>
-      <c r="F37" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K37" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="L37" s="33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="10" customFormat="1">
-      <c r="A38" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="C38" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="33" t="s">
-        <v>34</v>
-      </c>
       <c r="F38" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="G38" s="34"/>
+        <v>128</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>129</v>
+      </c>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
       <c r="J38" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K38" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="L38" s="33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="10" customFormat="1">
+        <v>130</v>
+      </c>
+      <c r="L38" s="33"/>
+    </row>
+    <row r="39" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="43" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C39" s="32" t="s">
         <v>14</v>
@@ -3113,7 +3149,7 @@
       </c>
       <c r="E39" s="33"/>
       <c r="F39" s="30" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
@@ -3122,18 +3158,18 @@
         <v>25</v>
       </c>
       <c r="K39" s="32" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="L39" s="33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="10" customFormat="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="42" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C40" s="32" t="s">
         <v>14</v>
@@ -3145,7 +3181,7 @@
         <v>34</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
@@ -3154,30 +3190,30 @@
         <v>19</v>
       </c>
       <c r="K40" s="32" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L40" s="33" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="10" customFormat="1">
-      <c r="A41" s="42" t="s">
-        <v>173</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="53" t="s">
+        <v>279</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>174</v>
+        <v>284</v>
       </c>
       <c r="C41" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E41" s="33" t="s">
         <v>34</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>151</v>
+        <v>272</v>
       </c>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
@@ -3186,18 +3222,18 @@
         <v>19</v>
       </c>
       <c r="K41" s="32" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L41" s="33" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="10" customFormat="1">
-      <c r="A42" s="42" t="s">
-        <v>175</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="43" t="s">
+        <v>281</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C42" s="32" t="s">
         <v>14</v>
@@ -3205,95 +3241,93 @@
       <c r="D42" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="33" t="s">
-        <v>61</v>
-      </c>
+      <c r="E42" s="33"/>
       <c r="F42" s="30" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="G42" s="34"/>
-      <c r="H42" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="I42" s="33" t="s">
-        <v>157</v>
-      </c>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
       <c r="J42" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K42" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="L42" s="33"/>
-    </row>
-    <row r="43" spans="1:12" s="10" customFormat="1">
+        <v>36</v>
+      </c>
+      <c r="L42" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="42" t="s">
-        <v>177</v>
+        <v>282</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C43" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>179</v>
+        <v>33</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="33" t="s">
-        <v>181</v>
-      </c>
+      <c r="I43" s="34"/>
       <c r="J43" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K43" s="32" t="s">
-        <v>133</v>
+        <v>43</v>
       </c>
       <c r="L43" s="33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="10" customFormat="1">
-      <c r="A44" s="52" t="s">
-        <v>183</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="42" t="s">
+        <v>283</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C44" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="33"/>
+      <c r="D44" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>34</v>
+      </c>
       <c r="F44" s="30" t="s">
-        <v>246</v>
+        <v>145</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
       <c r="J44" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K44" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="L44" s="33"/>
-    </row>
-    <row r="45" spans="1:12" s="10" customFormat="1">
+        <v>43</v>
+      </c>
+      <c r="L44" s="33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="42" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="C45" s="32" t="s">
         <v>14</v>
@@ -3302,503 +3336,599 @@
         <v>15</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>245</v>
+        <v>149</v>
       </c>
       <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
+      <c r="H45" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="I45" s="33" t="s">
+        <v>151</v>
+      </c>
       <c r="J45" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K45" s="32" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="L45" s="33"/>
     </row>
-    <row r="46" spans="1:12" s="10" customFormat="1">
+    <row r="46" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="42" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="C46" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F46" s="30" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
+      <c r="I46" s="33" t="s">
+        <v>172</v>
+      </c>
       <c r="J46" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K46" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="L46" s="33"/>
-    </row>
-    <row r="47" spans="1:12" s="10" customFormat="1">
-      <c r="A47" s="49" t="s">
-        <v>192</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47" s="60" t="s">
-        <v>196</v>
-      </c>
-      <c r="I47" s="12"/>
-      <c r="J47" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K47" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="L47" s="12"/>
-    </row>
-    <row r="48" spans="1:12" s="10" customFormat="1">
-      <c r="A48" s="53" t="s">
-        <v>240</v>
+        <v>130</v>
+      </c>
+      <c r="L46" s="33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="B47" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="33"/>
+      <c r="F47" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="L47" s="33"/>
+    </row>
+    <row r="48" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="42" t="s">
+        <v>176</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>241</v>
+        <v>177</v>
       </c>
       <c r="C48" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>242</v>
+        <v>15</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
-      <c r="I48" s="33" t="s">
-        <v>253</v>
-      </c>
+      <c r="I48" s="34"/>
       <c r="J48" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K48" s="32" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L48" s="33"/>
     </row>
-    <row r="49" spans="1:12" s="10" customFormat="1">
-      <c r="A49" s="52" t="s">
-        <v>197</v>
+    <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="42" t="s">
+        <v>180</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="C49" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E49" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="F49" s="30" t="s">
-        <v>247</v>
+        <v>182</v>
       </c>
       <c r="G49" s="34"/>
       <c r="H49" s="34"/>
       <c r="I49" s="34"/>
       <c r="J49" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K49" s="32" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="L49" s="33"/>
     </row>
-    <row r="50" spans="1:12" s="10" customFormat="1">
-      <c r="A50" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="B50" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="C50" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>244</v>
-      </c>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K50" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="L50" s="33"/>
-    </row>
-    <row r="51" spans="1:12" s="10" customFormat="1">
-      <c r="A51" s="42" t="s">
-        <v>202</v>
+    <row r="50" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="I50" s="12"/>
+      <c r="J50" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="L50" s="12"/>
+    </row>
+    <row r="51" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="53" t="s">
+        <v>231</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="C51" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>15</v>
+        <v>285</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>204</v>
+        <v>242</v>
       </c>
       <c r="G51" s="34"/>
       <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
+      <c r="I51" s="33" t="s">
+        <v>243</v>
+      </c>
       <c r="J51" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K51" s="32" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="L51" s="33"/>
     </row>
-    <row r="52" spans="1:12" s="10" customFormat="1">
-      <c r="A52" s="49" t="s">
-        <v>205</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="11" t="s">
+    <row r="52" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="33"/>
+      <c r="F52" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K52" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="L52" s="33"/>
+    </row>
+    <row r="53" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="L53" s="33"/>
+    </row>
+    <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="B54" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="E52" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F52" s="60" t="s">
-        <v>243</v>
-      </c>
-      <c r="I52" s="12"/>
-      <c r="J52" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K52" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="L52" s="12"/>
-    </row>
-    <row r="53" spans="1:12" s="50" customFormat="1" ht="15">
-      <c r="A53" s="54" t="s">
-        <v>255</v>
-      </c>
-      <c r="B53" s="50" t="s">
-        <v>257</v>
-      </c>
-      <c r="C53" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="50" t="s">
-        <v>260</v>
-      </c>
-      <c r="F53" s="62" t="s">
-        <v>261</v>
-      </c>
-      <c r="G53" s="57"/>
-      <c r="H53" s="57"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="K53" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="L53" s="58"/>
-    </row>
-    <row r="54" spans="1:12" s="10" customFormat="1">
-      <c r="A54" s="53" t="s">
-        <v>254</v>
-      </c>
-      <c r="B54" s="32" t="s">
-        <v>232</v>
-      </c>
       <c r="C54" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>258</v>
+        <v>15</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="G54" s="34"/>
       <c r="H54" s="34"/>
-      <c r="I54" s="33"/>
+      <c r="I54" s="34"/>
       <c r="J54" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K54" s="11" t="s">
-        <v>256</v>
+      <c r="K54" s="32" t="s">
+        <v>192</v>
       </c>
       <c r="L54" s="33"/>
     </row>
-    <row r="55" spans="1:12" s="10" customFormat="1">
-      <c r="A55" s="53" t="s">
-        <v>273</v>
-      </c>
-      <c r="B55" s="32" t="s">
-        <v>259</v>
-      </c>
-      <c r="C55" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="32" t="s">
-        <v>258</v>
-      </c>
-      <c r="E55" s="33"/>
-      <c r="F55" s="30" t="s">
-        <v>274</v>
-      </c>
-      <c r="G55" s="34"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="33"/>
-      <c r="J55" s="32" t="s">
+    <row r="55" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="I55" s="12"/>
+      <c r="J55" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="L55" s="33"/>
-    </row>
-    <row r="56" spans="1:12" s="10" customFormat="1">
-      <c r="A56" s="51" t="s">
-        <v>270</v>
-      </c>
-      <c r="B56" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="C56" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="32" t="s">
-        <v>258</v>
-      </c>
-      <c r="E56" s="33"/>
-      <c r="F56" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G56" s="34"/>
-      <c r="H56" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="I56" s="34"/>
-      <c r="J56" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="L55" s="12"/>
+    </row>
+    <row r="56" spans="1:12" s="50" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="54" t="s">
+        <v>245</v>
+      </c>
+      <c r="B56" s="50" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="F56" s="62" t="s">
+        <v>251</v>
+      </c>
+      <c r="G56" s="57"/>
+      <c r="H56" s="57"/>
+      <c r="I56" s="58"/>
+      <c r="J56" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="K56" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="L56" s="33"/>
-    </row>
-    <row r="57" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="A57" s="42" t="s">
-        <v>262</v>
+      <c r="K56" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="L56" s="58"/>
+    </row>
+    <row r="57" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="53" t="s">
+        <v>244</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="C57" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="E57" s="33" t="s">
         <v>16</v>
       </c>
       <c r="F57" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="G57" s="32" t="s">
-        <v>106</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="G57" s="34"/>
       <c r="H57" s="34"/>
-      <c r="I57" s="34"/>
+      <c r="I57" s="33"/>
       <c r="J57" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K57" s="32" t="s">
-        <v>107</v>
+      <c r="K57" s="11" t="s">
+        <v>246</v>
       </c>
       <c r="L57" s="33"/>
     </row>
-    <row r="58" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
-      <c r="A58" s="42" t="s">
+    <row r="58" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="53" t="s">
         <v>263</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="C58" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E58" s="33" t="s">
-        <v>34</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="E58" s="33"/>
       <c r="F58" s="30" t="s">
-        <v>110</v>
+        <v>264</v>
       </c>
       <c r="G58" s="34"/>
       <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
+      <c r="I58" s="33"/>
       <c r="J58" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K58" s="32" t="s">
+      <c r="K58" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="L58" s="33"/>
+    </row>
+    <row r="59" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="51" t="s">
+        <v>260</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="E59" s="33"/>
+      <c r="F59" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G59" s="34"/>
+      <c r="H59" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="I59" s="34"/>
+      <c r="J59" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K59" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="L59" s="33"/>
+    </row>
+    <row r="60" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="B60" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="E60" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K60" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L60" s="33"/>
+    </row>
+    <row r="61" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="B61" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F61" s="30" t="s">
         <v>107</v>
-      </c>
-      <c r="L58" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" s="10" customFormat="1">
-      <c r="A59" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="C59" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E59" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F59" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="G59" s="34"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="J59" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K59" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="L59" s="33"/>
-    </row>
-    <row r="60" spans="1:12" s="10" customFormat="1">
-      <c r="A60" s="49" t="s">
-        <v>264</v>
-      </c>
-      <c r="B60" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F60" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="J60" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K60" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L60" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="10" customFormat="1">
-      <c r="A61" s="54" t="s">
-        <v>234</v>
-      </c>
-      <c r="B61" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="C61" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E61" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" s="30" t="s">
-        <v>235</v>
       </c>
       <c r="G61" s="34"/>
       <c r="H61" s="34"/>
-      <c r="I61" s="33"/>
+      <c r="I61" s="34"/>
       <c r="J61" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K61" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="L61" s="33"/>
+      <c r="K61" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L61" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E62" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F62" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="J62" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K62" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L62" s="33"/>
+    </row>
+    <row r="63" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="B63" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F63" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K63" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="L63" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="B64" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K64" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L64" s="33"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N52" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}"/>
+  <autoFilter ref="A1:N55" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{21527874-0ADF-4209-82A0-BEEB3929A2FA}"/>
@@ -3807,130 +3937,136 @@
     <hyperlink ref="L3" r:id="rId4" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.6&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D2F9658F-C1BB-46F8-B14F-7F1E9A33F5D0}"/>
     <hyperlink ref="E4" r:id="rId5" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{2D6C3C97-4B85-40D6-BBEE-E84C287F4953}"/>
     <hyperlink ref="L4" r:id="rId6" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.287&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8052636D-92E8-47F8-8501-468D86170759}"/>
-    <hyperlink ref="E5" r:id="rId7" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{6082C308-02AA-4F93-A532-4965FE9AA0D2}"/>
-    <hyperlink ref="L5" r:id="rId8" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.291&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{BC26797E-423D-486B-99BC-93D45C79BCCA}"/>
-    <hyperlink ref="E6" r:id="rId9" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{E616D0B0-9679-48B8-B0B5-DEAA377935F3}"/>
-    <hyperlink ref="L6" r:id="rId10" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.292&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A32CE57D-BD57-44A2-9845-8A4D09951F84}"/>
-    <hyperlink ref="E7" r:id="rId11" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{0551098E-9234-4D8A-B330-3BA56EB1A481}"/>
-    <hyperlink ref="L7" r:id="rId12" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.293&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3A48A772-C277-4FC8-A729-B03D0C7B85E3}"/>
-    <hyperlink ref="E8" r:id="rId13" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{CB05C4C7-5AA6-482F-B5DB-F86F2DB5A99D}"/>
-    <hyperlink ref="L8" r:id="rId14" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3511378B-C826-4D18-A4AD-9D763E598C21}"/>
-    <hyperlink ref="E10" r:id="rId15" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{A88DB6BD-5A02-4441-89C5-520010EAB2F3}"/>
-    <hyperlink ref="I10" r:id="rId16" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.0.1.1&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{9568874B-352E-4F05-8F9B-6BE21E0CE6DF}"/>
-    <hyperlink ref="L10" r:id="rId17" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.9&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{B07B20EC-EEA0-4A1D-94EE-202E9BCAB8AE}"/>
-    <hyperlink ref="E11" r:id="rId18" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{922A599D-1B97-49FD-87DF-4C89C8A50B9A}"/>
-    <hyperlink ref="L11" r:id="rId19" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{583E6F9B-6DB0-46D1-9745-78B6C9391490}"/>
-    <hyperlink ref="E12" r:id="rId20" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{70575BDC-3CBF-4D19-840E-D4F9DCDD9611}"/>
-    <hyperlink ref="H12" r:id="rId21" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=71388002&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{BFD34CA0-A9C0-4878-B96E-15D6961A4708}"/>
-    <hyperlink ref="L12" r:id="rId22" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{F924C40E-13C1-4545-B359-5C38B9E50843}"/>
-    <hyperlink ref="E13" r:id="rId23" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{4F369B33-4E33-401E-93B5-2E8FCA323C37}"/>
-    <hyperlink ref="L13" r:id="rId24" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4FBBD0B5-A85C-47DB-ADE9-26726662ED0A}"/>
-    <hyperlink ref="E14" r:id="rId25" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{D55F35D2-5945-43D7-883D-14F1980F60DE}"/>
-    <hyperlink ref="L14" r:id="rId26" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.14.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{ADCBB6A1-F352-49A6-90A4-3227DC51BFA3}"/>
-    <hyperlink ref="E15" r:id="rId27" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{A9242079-E6F4-440E-AA0D-C7AC227BA891}"/>
-    <hyperlink ref="I15" r:id="rId28" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.133.11.1&amp;effectiveDate=2023-08-08T11:35:39&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{DCE428FB-F940-478E-9AD6-F712BBCF1368}"/>
-    <hyperlink ref="L15" r:id="rId29" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0F5EEFBE-EF1B-436D-8153-1DF37092F09B}"/>
-    <hyperlink ref="E16" r:id="rId30" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{1860309C-57AB-4C44-87F5-3CFC1E7AA68C}"/>
-    <hyperlink ref="H16" r:id="rId31" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=405813007&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{96482A48-8D77-49BF-A4A3-0877A32F22A3}"/>
-    <hyperlink ref="L16" r:id="rId32" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8BBD944A-1BBF-41DD-9895-47A3F8A016CB}"/>
-    <hyperlink ref="E19" r:id="rId33" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{0B105CE1-A24B-48E9-B64A-10CC194A7E35}"/>
-    <hyperlink ref="L19" r:id="rId34" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{C0D00567-AFBA-4261-A1D6-28C14041C6EB}"/>
-    <hyperlink ref="E20" r:id="rId35" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{BED85187-1744-44AD-BC59-4031E9D51ACA}"/>
-    <hyperlink ref="H20" r:id="rId36" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{F52E0121-2128-4409-A848-24A442B7BE12}"/>
-    <hyperlink ref="L20" r:id="rId37" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{CE49BD0D-FB2A-4C55-A43F-3CB4371BF5DA}"/>
-    <hyperlink ref="E21" r:id="rId38" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{C4207001-6F30-4D74-9216-927CE59A5BDB}"/>
-    <hyperlink ref="L21" r:id="rId39" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5F752677-153F-481E-A065-AEA95290C150}"/>
-    <hyperlink ref="E22" r:id="rId40" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{91C4C455-EE40-44B4-AFDA-F862EC72BBD6}"/>
-    <hyperlink ref="L22" r:id="rId41" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D8C3E848-E1AF-4099-868D-E376521C25BF}"/>
-    <hyperlink ref="E23" r:id="rId42" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{418DEEFE-D67D-4689-A6E4-8CCA2C059267}"/>
-    <hyperlink ref="I23" r:id="rId43" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.106.11.22&amp;effectiveDate=2024-02-05T13:30:06&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{98A2B0FA-9C5E-4835-8C61-1A0CC6C56CDA}"/>
-    <hyperlink ref="L23" r:id="rId44" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{AB70A3AA-2A28-4B85-9441-772C138D4B6E}"/>
-    <hyperlink ref="E34" r:id="rId45" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{AA591DB2-7581-46E2-B467-F49155C3C44F}"/>
-    <hyperlink ref="L34" r:id="rId46" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{7A6D0C4C-D2DB-43F9-993C-E3BD7CAD92DD}"/>
-    <hyperlink ref="E35" r:id="rId47" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{0E5CACCC-3BC7-45ED-A665-4B961B6B79FD}"/>
-    <hyperlink ref="H35" r:id="rId48" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=223366009&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{5DB75BFC-D55E-4875-A437-1E620AD1ACE4}"/>
-    <hyperlink ref="L35" r:id="rId49" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0DAFCDC1-3A35-49F9-86A3-EFCE8351E49C}"/>
-    <hyperlink ref="E36" r:id="rId50" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{0F8E1113-3C1F-4098-81AA-D103A3C3E4E1}"/>
-    <hyperlink ref="L36" r:id="rId51" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{889B9854-48EA-4632-81DD-4C6AC8341069}"/>
-    <hyperlink ref="E37" r:id="rId52" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{FD23A05B-2D6F-4CA6-A620-B9D2C5766B78}"/>
-    <hyperlink ref="L37" r:id="rId53" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{926D7745-EF2D-49AD-8F64-AF74702980F3}"/>
-    <hyperlink ref="E38" r:id="rId54" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{463D1E76-10B0-45B7-9680-F5B3B24CC195}"/>
-    <hyperlink ref="L38" r:id="rId55" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.496&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E699B27A-3C84-4DC0-9C6D-C87DFA62EFCD}"/>
-    <hyperlink ref="E39" r:id="rId56" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{21E08D7F-CC64-4EFD-8211-99F5A0A92B3A}"/>
-    <hyperlink ref="L39" r:id="rId57" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.500&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0A4D7A71-024C-4B56-BF9D-06312EDDFF1C}"/>
-    <hyperlink ref="E40" r:id="rId58" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{AD3E600D-6354-4484-B4CE-1CF836CB3054}"/>
-    <hyperlink ref="L40" r:id="rId59" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.501&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{56CCB389-1A8A-4EEA-A783-B92FD345BEA7}"/>
-    <hyperlink ref="E41" r:id="rId60" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{11838974-4C55-46FA-92B4-A485B6B64428}"/>
-    <hyperlink ref="L41" r:id="rId61" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.502&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D871510D-E999-4D2C-99D0-04BF1F5FDF41}"/>
-    <hyperlink ref="E44" r:id="rId62" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{9B4581F7-385E-4379-9BEE-02A167F1905B}"/>
-    <hyperlink ref="L44" r:id="rId63" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{DFCED3FF-24D8-40A9-B08F-9E70FA3370B3}"/>
-    <hyperlink ref="E45" r:id="rId64" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{F7ED96CE-5F04-4A4D-99A2-7537C3B8214B}"/>
-    <hyperlink ref="L45" r:id="rId65" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{315742DA-B29B-4B38-8898-713230484F64}"/>
-    <hyperlink ref="E46" r:id="rId66" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{1DD7FB21-ADBA-43A1-8D64-769C58250348}"/>
-    <hyperlink ref="L46" r:id="rId67" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{81FECE2A-75A0-4F3C-B166-B8CF5C058228}"/>
-    <hyperlink ref="E49" r:id="rId68" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{49D5FF9B-FE40-43A6-A865-3F174F2030FA}"/>
-    <hyperlink ref="L49" r:id="rId69" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4FAB496D-24B1-47A2-A9A0-9552D567398B}"/>
-    <hyperlink ref="E50" r:id="rId70" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7B8E1B66-0D74-498D-8D88-C6351C4F7FB1}"/>
-    <hyperlink ref="L50" r:id="rId71" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E05351A4-8368-4A4B-B12F-961BE504A1A5}"/>
-    <hyperlink ref="E51" r:id="rId72" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{B9A776CF-FC80-4D4E-9655-984F31074E85}"/>
-    <hyperlink ref="L51" r:id="rId73" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A19CC1FA-FBE7-46A2-A89E-FC0E605879FD}"/>
-    <hyperlink ref="L24" r:id="rId74" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.4&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{6F907670-FA22-4633-9957-BF1722D97459}"/>
-    <hyperlink ref="I24" r:id="rId75" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.2.3&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A620A0BE-0D93-418C-8E02-69F661FAE5FD}"/>
-    <hyperlink ref="E24" r:id="rId76" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{6429EA44-A0BE-46EC-BF67-7430BB9AAE0F}"/>
-    <hyperlink ref="E43" r:id="rId77" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{210AF206-8EC6-4753-B18F-691F0E018F4B}"/>
-    <hyperlink ref="I43" r:id="rId78" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.5&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A6DE206C-E455-40DC-9E1B-756F49B6FF18}"/>
-    <hyperlink ref="L43" r:id="rId79" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.5&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{15507FCB-F9AC-4DBB-8436-76E49E25C5EF}"/>
-    <hyperlink ref="L42" r:id="rId80" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8E324497-0C3B-4040-AC01-896E177058B3}"/>
-    <hyperlink ref="I42" r:id="rId81" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.6&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CA8E4A7-71BA-4090-8600-26CBB7FEFE64}"/>
-    <hyperlink ref="H42" r:id="rId82" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=394658006&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{721ECB08-9ED5-4D83-9D6F-3E36BCB4E97A}"/>
-    <hyperlink ref="E42" r:id="rId83" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{171680EF-1354-4A0A-B685-C2521C9E7B5B}"/>
-    <hyperlink ref="I23" r:id="rId84" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.17.2.4/2020-09-01T00:00:00" xr:uid="{3BC999B2-E1FF-764B-A460-2EFE8CF33320}"/>
-    <hyperlink ref="E9" r:id="rId85" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{901B3EB5-29F2-4EB0-906C-663F0E4F00B7}"/>
-    <hyperlink ref="L9" r:id="rId86" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.10&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0BB30E11-298C-4DA7-981F-84CAA9D1E49F}"/>
-    <hyperlink ref="H19" r:id="rId87" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{2F46476A-CCBE-47CE-83E8-8C15158702E5}"/>
-    <hyperlink ref="E25" r:id="rId88" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{2EFAD0E2-EF39-4D43-934D-C9B1B5EC46FD}"/>
-    <hyperlink ref="L25" r:id="rId89" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E5CB3AF8-CD35-4336-A52E-F1CD36342B9A}"/>
-    <hyperlink ref="E26" r:id="rId90" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{157CAA35-1F3A-4644-9743-0D3BD7B1AD5D}"/>
-    <hyperlink ref="H26" r:id="rId91" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=223366009&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{B6C54458-5BA4-4CA8-A9E2-5C243DCAF8C7}"/>
-    <hyperlink ref="L26" r:id="rId92" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{400D9654-7241-454F-B4F1-DB0BBFC28C7F}"/>
-    <hyperlink ref="E27" r:id="rId93" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7A911ED1-456E-42DD-8989-6C37E008CB8F}"/>
-    <hyperlink ref="L27" r:id="rId94" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5CD64B4F-E83F-4005-9A6E-787F3DB78C1F}"/>
-    <hyperlink ref="E28" r:id="rId95" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{78F78CB4-BF12-439E-A376-A5EFEAB9638A}"/>
-    <hyperlink ref="L28" r:id="rId96" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{C9A85D4A-8788-4DF9-97F9-4EB018D4A5B9}"/>
-    <hyperlink ref="E29" r:id="rId97" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{71892660-7F1C-472A-B162-6A37867B13E4}"/>
-    <hyperlink ref="L29" r:id="rId98" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.496&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D5BD9CA3-83A5-49DA-8EDA-EECAF1D8A30A}"/>
-    <hyperlink ref="E30" r:id="rId99" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{A1C783D9-54A1-47F4-8609-B81B79B0BCAC}"/>
-    <hyperlink ref="L30" r:id="rId100" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.500&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{CBF81741-6FE3-47AD-A8C5-5D921B4024A1}"/>
-    <hyperlink ref="E31" r:id="rId101" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{32C938FB-EABD-4ECA-A7CE-58F10B8BE3B9}"/>
-    <hyperlink ref="L31" r:id="rId102" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.501&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8485E509-F6A8-4CBD-8193-E802481F42A7}"/>
-    <hyperlink ref="E32" r:id="rId103" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{1505873D-5C29-4DF7-8109-CAA50E5FEC45}"/>
-    <hyperlink ref="L32" r:id="rId104" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.502&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{085BE848-B522-4E53-98CC-F69378ED9E7C}"/>
-    <hyperlink ref="L33" r:id="rId105" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4A02E4C8-6668-4133-8C05-A005AE0BC874}"/>
-    <hyperlink ref="I33" r:id="rId106" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.6&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{44E6768D-4906-4177-B6A3-F069389C6FAC}"/>
-    <hyperlink ref="H33" r:id="rId107" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=394658006&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{1EA9AE6D-E4A5-489E-A391-5105421A577E}"/>
-    <hyperlink ref="E33" r:id="rId108" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{412E7912-214B-462C-9DA8-FB6F7B146124}"/>
-    <hyperlink ref="L17" r:id="rId109" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5C01C431-F32A-497B-92D2-4D058995BE9E}"/>
-    <hyperlink ref="I17" r:id="rId110" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.106.11.19&amp;effectiveDate=2024-02-05T12:33:45&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D71DB53F-4DFA-456E-A6FD-A94C4290D1C1}"/>
-    <hyperlink ref="H17" r:id="rId111" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=363698007&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{58172FD2-70FC-4673-BF70-D6AE18467415}"/>
-    <hyperlink ref="E17" r:id="rId112" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{3D0023D3-652A-4840-9808-3B2E5DA099D0}"/>
-    <hyperlink ref="E18" r:id="rId113" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.20.7.2/2020-09-01T00:00:00" xr:uid="{4B3833E8-D6ED-4EC3-8D1E-0F1FF55B206E}"/>
-    <hyperlink ref="E54" r:id="rId114" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{06898B6A-A0ED-0244-9A16-72B56DEBED42}"/>
-    <hyperlink ref="E61" r:id="rId115" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{EABED256-857D-2642-BE3E-5AD20C03336E}"/>
-    <hyperlink ref="E48" r:id="rId116" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{0BB16F56-88D4-5644-B710-8B7860CB1712}"/>
-    <hyperlink ref="I48" r:id="rId117" xr:uid="{E48A8B75-06B7-5444-866E-89BA6FC9A9FC}"/>
-    <hyperlink ref="E56" r:id="rId118" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{24C31C8F-A2E9-824A-9317-3AA15CB5B012}"/>
-    <hyperlink ref="H56" r:id="rId119" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{C869B80E-2110-5741-BB09-F7EDBF5A7FAE}"/>
-    <hyperlink ref="L56" r:id="rId120" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D915B272-925A-FB46-A898-7CF03503B973}"/>
-    <hyperlink ref="E57" r:id="rId121" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{D7AA8219-AC02-7D4E-9C12-CABC33799EC4}"/>
-    <hyperlink ref="L57" r:id="rId122" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3965CB55-85FB-5D4E-B610-010B1CD32274}"/>
-    <hyperlink ref="E58" r:id="rId123" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{93663DF7-6AD3-2748-912C-FCEE1C2CC562}"/>
-    <hyperlink ref="L58" r:id="rId124" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{F63D6C9B-9ACA-A348-B301-C940CA72AF2C}"/>
-    <hyperlink ref="E59" r:id="rId125" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{F351B801-B480-8645-9B04-58FF53EFC89A}"/>
-    <hyperlink ref="I59" r:id="rId126" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.17.2.4/2020-09-01T00:00:00" xr:uid="{8DDE88C1-182D-284E-AF9A-5977BFBB50BA}"/>
-    <hyperlink ref="L59" r:id="rId127" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{41CE1CBD-75FF-1547-A9BA-108D0AB0450D}"/>
-    <hyperlink ref="L60" r:id="rId128" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.4&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{87455DB6-3D09-9849-9FC5-EBE0AF4C3CEA}"/>
-    <hyperlink ref="I60" r:id="rId129" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.2.3&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{B5CE4245-F76E-3B42-ADA9-69F1DC52B3D6}"/>
-    <hyperlink ref="E60" r:id="rId130" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{7BF95595-025E-BE48-94C3-E19456DD2154}"/>
+    <hyperlink ref="E6" r:id="rId7" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{6082C308-02AA-4F93-A532-4965FE9AA0D2}"/>
+    <hyperlink ref="L6" r:id="rId8" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.291&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{BC26797E-423D-486B-99BC-93D45C79BCCA}"/>
+    <hyperlink ref="E7" r:id="rId9" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{E616D0B0-9679-48B8-B0B5-DEAA377935F3}"/>
+    <hyperlink ref="L7" r:id="rId10" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.292&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A32CE57D-BD57-44A2-9845-8A4D09951F84}"/>
+    <hyperlink ref="E8" r:id="rId11" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{0551098E-9234-4D8A-B330-3BA56EB1A481}"/>
+    <hyperlink ref="L8" r:id="rId12" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.293&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3A48A772-C277-4FC8-A729-B03D0C7B85E3}"/>
+    <hyperlink ref="E9" r:id="rId13" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{CB05C4C7-5AA6-482F-B5DB-F86F2DB5A99D}"/>
+    <hyperlink ref="L9" r:id="rId14" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3511378B-C826-4D18-A4AD-9D763E598C21}"/>
+    <hyperlink ref="E11" r:id="rId15" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{A88DB6BD-5A02-4441-89C5-520010EAB2F3}"/>
+    <hyperlink ref="I11" r:id="rId16" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.0.1.1&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{9568874B-352E-4F05-8F9B-6BE21E0CE6DF}"/>
+    <hyperlink ref="L11" r:id="rId17" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.9&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{B07B20EC-EEA0-4A1D-94EE-202E9BCAB8AE}"/>
+    <hyperlink ref="E12" r:id="rId18" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{922A599D-1B97-49FD-87DF-4C89C8A50B9A}"/>
+    <hyperlink ref="L12" r:id="rId19" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{583E6F9B-6DB0-46D1-9745-78B6C9391490}"/>
+    <hyperlink ref="E13" r:id="rId20" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{70575BDC-3CBF-4D19-840E-D4F9DCDD9611}"/>
+    <hyperlink ref="H13" r:id="rId21" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=71388002&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{BFD34CA0-A9C0-4878-B96E-15D6961A4708}"/>
+    <hyperlink ref="L13" r:id="rId22" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{F924C40E-13C1-4545-B359-5C38B9E50843}"/>
+    <hyperlink ref="E14" r:id="rId23" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{4F369B33-4E33-401E-93B5-2E8FCA323C37}"/>
+    <hyperlink ref="L14" r:id="rId24" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4FBBD0B5-A85C-47DB-ADE9-26726662ED0A}"/>
+    <hyperlink ref="E15" r:id="rId25" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{D55F35D2-5945-43D7-883D-14F1980F60DE}"/>
+    <hyperlink ref="L15" r:id="rId26" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.14.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{ADCBB6A1-F352-49A6-90A4-3227DC51BFA3}"/>
+    <hyperlink ref="E16" r:id="rId27" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{A9242079-E6F4-440E-AA0D-C7AC227BA891}"/>
+    <hyperlink ref="I16" r:id="rId28" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.133.11.1&amp;effectiveDate=2023-08-08T11:35:39&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{DCE428FB-F940-478E-9AD6-F712BBCF1368}"/>
+    <hyperlink ref="L16" r:id="rId29" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0F5EEFBE-EF1B-436D-8153-1DF37092F09B}"/>
+    <hyperlink ref="E17" r:id="rId30" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{1860309C-57AB-4C44-87F5-3CFC1E7AA68C}"/>
+    <hyperlink ref="H17" r:id="rId31" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=405813007&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{96482A48-8D77-49BF-A4A3-0877A32F22A3}"/>
+    <hyperlink ref="L17" r:id="rId32" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8BBD944A-1BBF-41DD-9895-47A3F8A016CB}"/>
+    <hyperlink ref="E20" r:id="rId33" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{0B105CE1-A24B-48E9-B64A-10CC194A7E35}"/>
+    <hyperlink ref="L20" r:id="rId34" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{C0D00567-AFBA-4261-A1D6-28C14041C6EB}"/>
+    <hyperlink ref="E21" r:id="rId35" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{BED85187-1744-44AD-BC59-4031E9D51ACA}"/>
+    <hyperlink ref="H21" r:id="rId36" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{F52E0121-2128-4409-A848-24A442B7BE12}"/>
+    <hyperlink ref="L21" r:id="rId37" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{CE49BD0D-FB2A-4C55-A43F-3CB4371BF5DA}"/>
+    <hyperlink ref="E22" r:id="rId38" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{C4207001-6F30-4D74-9216-927CE59A5BDB}"/>
+    <hyperlink ref="L22" r:id="rId39" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5F752677-153F-481E-A065-AEA95290C150}"/>
+    <hyperlink ref="E23" r:id="rId40" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{91C4C455-EE40-44B4-AFDA-F862EC72BBD6}"/>
+    <hyperlink ref="L23" r:id="rId41" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D8C3E848-E1AF-4099-868D-E376521C25BF}"/>
+    <hyperlink ref="E24" r:id="rId42" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{418DEEFE-D67D-4689-A6E4-8CCA2C059267}"/>
+    <hyperlink ref="I24" r:id="rId43" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.106.11.22&amp;effectiveDate=2024-02-05T13:30:06&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{98A2B0FA-9C5E-4835-8C61-1A0CC6C56CDA}"/>
+    <hyperlink ref="L24" r:id="rId44" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{AB70A3AA-2A28-4B85-9441-772C138D4B6E}"/>
+    <hyperlink ref="E36" r:id="rId45" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{AA591DB2-7581-46E2-B467-F49155C3C44F}"/>
+    <hyperlink ref="L36" r:id="rId46" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{7A6D0C4C-D2DB-43F9-993C-E3BD7CAD92DD}"/>
+    <hyperlink ref="E37" r:id="rId47" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{0E5CACCC-3BC7-45ED-A665-4B961B6B79FD}"/>
+    <hyperlink ref="H37" r:id="rId48" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=223366009&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{5DB75BFC-D55E-4875-A437-1E620AD1ACE4}"/>
+    <hyperlink ref="L37" r:id="rId49" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0DAFCDC1-3A35-49F9-86A3-EFCE8351E49C}"/>
+    <hyperlink ref="E38" r:id="rId50" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{0F8E1113-3C1F-4098-81AA-D103A3C3E4E1}"/>
+    <hyperlink ref="L38" r:id="rId51" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{889B9854-48EA-4632-81DD-4C6AC8341069}"/>
+    <hyperlink ref="E39" r:id="rId52" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{FD23A05B-2D6F-4CA6-A620-B9D2C5766B78}"/>
+    <hyperlink ref="L39" r:id="rId53" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{926D7745-EF2D-49AD-8F64-AF74702980F3}"/>
+    <hyperlink ref="E40" r:id="rId54" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{463D1E76-10B0-45B7-9680-F5B3B24CC195}"/>
+    <hyperlink ref="L40" r:id="rId55" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.496&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E699B27A-3C84-4DC0-9C6D-C87DFA62EFCD}"/>
+    <hyperlink ref="E42" r:id="rId56" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{21E08D7F-CC64-4EFD-8211-99F5A0A92B3A}"/>
+    <hyperlink ref="L42" r:id="rId57" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.500&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0A4D7A71-024C-4B56-BF9D-06312EDDFF1C}"/>
+    <hyperlink ref="E43" r:id="rId58" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{AD3E600D-6354-4484-B4CE-1CF836CB3054}"/>
+    <hyperlink ref="L43" r:id="rId59" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.501&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{56CCB389-1A8A-4EEA-A783-B92FD345BEA7}"/>
+    <hyperlink ref="E44" r:id="rId60" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{11838974-4C55-46FA-92B4-A485B6B64428}"/>
+    <hyperlink ref="L44" r:id="rId61" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.502&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D871510D-E999-4D2C-99D0-04BF1F5FDF41}"/>
+    <hyperlink ref="E47" r:id="rId62" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{9B4581F7-385E-4379-9BEE-02A167F1905B}"/>
+    <hyperlink ref="L47" r:id="rId63" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{DFCED3FF-24D8-40A9-B08F-9E70FA3370B3}"/>
+    <hyperlink ref="E48" r:id="rId64" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{F7ED96CE-5F04-4A4D-99A2-7537C3B8214B}"/>
+    <hyperlink ref="L48" r:id="rId65" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{315742DA-B29B-4B38-8898-713230484F64}"/>
+    <hyperlink ref="E49" r:id="rId66" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{1DD7FB21-ADBA-43A1-8D64-769C58250348}"/>
+    <hyperlink ref="L49" r:id="rId67" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{81FECE2A-75A0-4F3C-B166-B8CF5C058228}"/>
+    <hyperlink ref="E52" r:id="rId68" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{49D5FF9B-FE40-43A6-A865-3F174F2030FA}"/>
+    <hyperlink ref="L52" r:id="rId69" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4FAB496D-24B1-47A2-A9A0-9552D567398B}"/>
+    <hyperlink ref="E53" r:id="rId70" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7B8E1B66-0D74-498D-8D88-C6351C4F7FB1}"/>
+    <hyperlink ref="L53" r:id="rId71" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E05351A4-8368-4A4B-B12F-961BE504A1A5}"/>
+    <hyperlink ref="E54" r:id="rId72" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{B9A776CF-FC80-4D4E-9655-984F31074E85}"/>
+    <hyperlink ref="L54" r:id="rId73" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A19CC1FA-FBE7-46A2-A89E-FC0E605879FD}"/>
+    <hyperlink ref="L25" r:id="rId74" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.4&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{6F907670-FA22-4633-9957-BF1722D97459}"/>
+    <hyperlink ref="I25" r:id="rId75" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.2.3&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A620A0BE-0D93-418C-8E02-69F661FAE5FD}"/>
+    <hyperlink ref="E25" r:id="rId76" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{6429EA44-A0BE-46EC-BF67-7430BB9AAE0F}"/>
+    <hyperlink ref="E46" r:id="rId77" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{210AF206-8EC6-4753-B18F-691F0E018F4B}"/>
+    <hyperlink ref="I46" r:id="rId78" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.5&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A6DE206C-E455-40DC-9E1B-756F49B6FF18}"/>
+    <hyperlink ref="L46" r:id="rId79" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.5&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{15507FCB-F9AC-4DBB-8436-76E49E25C5EF}"/>
+    <hyperlink ref="L45" r:id="rId80" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8E324497-0C3B-4040-AC01-896E177058B3}"/>
+    <hyperlink ref="I45" r:id="rId81" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.6&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CA8E4A7-71BA-4090-8600-26CBB7FEFE64}"/>
+    <hyperlink ref="H45" r:id="rId82" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=394658006&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{721ECB08-9ED5-4D83-9D6F-3E36BCB4E97A}"/>
+    <hyperlink ref="E45" r:id="rId83" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{171680EF-1354-4A0A-B685-C2521C9E7B5B}"/>
+    <hyperlink ref="I24" r:id="rId84" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.17.2.4/2020-09-01T00:00:00" xr:uid="{3BC999B2-E1FF-764B-A460-2EFE8CF33320}"/>
+    <hyperlink ref="E10" r:id="rId85" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{901B3EB5-29F2-4EB0-906C-663F0E4F00B7}"/>
+    <hyperlink ref="L10" r:id="rId86" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.10&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0BB30E11-298C-4DA7-981F-84CAA9D1E49F}"/>
+    <hyperlink ref="H20" r:id="rId87" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{2F46476A-CCBE-47CE-83E8-8C15158702E5}"/>
+    <hyperlink ref="E26" r:id="rId88" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{2EFAD0E2-EF39-4D43-934D-C9B1B5EC46FD}"/>
+    <hyperlink ref="L26" r:id="rId89" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E5CB3AF8-CD35-4336-A52E-F1CD36342B9A}"/>
+    <hyperlink ref="E27" r:id="rId90" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{157CAA35-1F3A-4644-9743-0D3BD7B1AD5D}"/>
+    <hyperlink ref="H27" r:id="rId91" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=223366009&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{B6C54458-5BA4-4CA8-A9E2-5C243DCAF8C7}"/>
+    <hyperlink ref="L27" r:id="rId92" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{400D9654-7241-454F-B4F1-DB0BBFC28C7F}"/>
+    <hyperlink ref="E28" r:id="rId93" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7A911ED1-456E-42DD-8989-6C37E008CB8F}"/>
+    <hyperlink ref="L28" r:id="rId94" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5CD64B4F-E83F-4005-9A6E-787F3DB78C1F}"/>
+    <hyperlink ref="E29" r:id="rId95" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{78F78CB4-BF12-439E-A376-A5EFEAB9638A}"/>
+    <hyperlink ref="L29" r:id="rId96" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{C9A85D4A-8788-4DF9-97F9-4EB018D4A5B9}"/>
+    <hyperlink ref="E30" r:id="rId97" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{71892660-7F1C-472A-B162-6A37867B13E4}"/>
+    <hyperlink ref="L30" r:id="rId98" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.496&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D5BD9CA3-83A5-49DA-8EDA-EECAF1D8A30A}"/>
+    <hyperlink ref="E32" r:id="rId99" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{A1C783D9-54A1-47F4-8609-B81B79B0BCAC}"/>
+    <hyperlink ref="L32" r:id="rId100" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.500&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{CBF81741-6FE3-47AD-A8C5-5D921B4024A1}"/>
+    <hyperlink ref="E33" r:id="rId101" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{32C938FB-EABD-4ECA-A7CE-58F10B8BE3B9}"/>
+    <hyperlink ref="L33" r:id="rId102" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.501&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8485E509-F6A8-4CBD-8193-E802481F42A7}"/>
+    <hyperlink ref="E34" r:id="rId103" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{1505873D-5C29-4DF7-8109-CAA50E5FEC45}"/>
+    <hyperlink ref="L34" r:id="rId104" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.502&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{085BE848-B522-4E53-98CC-F69378ED9E7C}"/>
+    <hyperlink ref="L35" r:id="rId105" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4A02E4C8-6668-4133-8C05-A005AE0BC874}"/>
+    <hyperlink ref="I35" r:id="rId106" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.6&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{44E6768D-4906-4177-B6A3-F069389C6FAC}"/>
+    <hyperlink ref="H35" r:id="rId107" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=394658006&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{1EA9AE6D-E4A5-489E-A391-5105421A577E}"/>
+    <hyperlink ref="E35" r:id="rId108" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{412E7912-214B-462C-9DA8-FB6F7B146124}"/>
+    <hyperlink ref="L18" r:id="rId109" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5C01C431-F32A-497B-92D2-4D058995BE9E}"/>
+    <hyperlink ref="I18" r:id="rId110" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.106.11.19&amp;effectiveDate=2024-02-05T12:33:45&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D71DB53F-4DFA-456E-A6FD-A94C4290D1C1}"/>
+    <hyperlink ref="H18" r:id="rId111" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=363698007&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{58172FD2-70FC-4673-BF70-D6AE18467415}"/>
+    <hyperlink ref="E18" r:id="rId112" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{3D0023D3-652A-4840-9808-3B2E5DA099D0}"/>
+    <hyperlink ref="E19" r:id="rId113" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.20.7.2/2020-09-01T00:00:00" xr:uid="{4B3833E8-D6ED-4EC3-8D1E-0F1FF55B206E}"/>
+    <hyperlink ref="E57" r:id="rId114" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{06898B6A-A0ED-0244-9A16-72B56DEBED42}"/>
+    <hyperlink ref="E64" r:id="rId115" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{EABED256-857D-2642-BE3E-5AD20C03336E}"/>
+    <hyperlink ref="E51" r:id="rId116" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{0BB16F56-88D4-5644-B710-8B7860CB1712}"/>
+    <hyperlink ref="I51" r:id="rId117" xr:uid="{E48A8B75-06B7-5444-866E-89BA6FC9A9FC}"/>
+    <hyperlink ref="E59" r:id="rId118" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{24C31C8F-A2E9-824A-9317-3AA15CB5B012}"/>
+    <hyperlink ref="H59" r:id="rId119" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{C869B80E-2110-5741-BB09-F7EDBF5A7FAE}"/>
+    <hyperlink ref="L59" r:id="rId120" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D915B272-925A-FB46-A898-7CF03503B973}"/>
+    <hyperlink ref="E60" r:id="rId121" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{D7AA8219-AC02-7D4E-9C12-CABC33799EC4}"/>
+    <hyperlink ref="L60" r:id="rId122" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3965CB55-85FB-5D4E-B610-010B1CD32274}"/>
+    <hyperlink ref="E61" r:id="rId123" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{93663DF7-6AD3-2748-912C-FCEE1C2CC562}"/>
+    <hyperlink ref="L61" r:id="rId124" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{F63D6C9B-9ACA-A348-B301-C940CA72AF2C}"/>
+    <hyperlink ref="E62" r:id="rId125" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{F351B801-B480-8645-9B04-58FF53EFC89A}"/>
+    <hyperlink ref="I62" r:id="rId126" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.17.2.4/2020-09-01T00:00:00" xr:uid="{8DDE88C1-182D-284E-AF9A-5977BFBB50BA}"/>
+    <hyperlink ref="L62" r:id="rId127" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{41CE1CBD-75FF-1547-A9BA-108D0AB0450D}"/>
+    <hyperlink ref="L63" r:id="rId128" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.4&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{87455DB6-3D09-9849-9FC5-EBE0AF4C3CEA}"/>
+    <hyperlink ref="I63" r:id="rId129" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.2.3&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{B5CE4245-F76E-3B42-ADA9-69F1DC52B3D6}"/>
+    <hyperlink ref="E63" r:id="rId130" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{7BF95595-025E-BE48-94C3-E19456DD2154}"/>
+    <hyperlink ref="E5" r:id="rId131" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{97B37183-E333-2F40-A93B-078DC30E8909}"/>
+    <hyperlink ref="L5" r:id="rId132" xr:uid="{3C80AA13-A8C0-DB4D-B55B-11C3AC1DD645}"/>
+    <hyperlink ref="E31" r:id="rId133" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{7C87E736-C37B-AD4E-8676-0CEC0731A8C6}"/>
+    <hyperlink ref="L31" r:id="rId134" xr:uid="{AB99BCA2-5B5E-A84E-9445-25F8993321E0}"/>
+    <hyperlink ref="E41" r:id="rId135" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{8E5A2DA5-3A93-9B4F-96B8-A9C383954120}"/>
+    <hyperlink ref="L41" r:id="rId136" xr:uid="{14E761D3-2F17-284C-B1F3-C5DA9DA1930D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3944,13 +4080,13 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3973,7 +4109,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -3988,7 +4124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -4021,12 +4157,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>14</v>
@@ -4038,23 +4174,23 @@
         <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="H3" s="28"/>
       <c r="J3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1">
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
@@ -4066,14 +4202,14 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="H4" s="27"/>
       <c r="J4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L4" s="3"/>
     </row>
@@ -4092,13 +4228,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A01627-17D2-4A39-A8A2-B1EFC11356BF}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="17" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -4107,7 +4243,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4145,9 +4281,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>23</v>
@@ -4169,7 +4305,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1">
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>27</v>
       </c>
@@ -4196,7 +4332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1">
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -4225,97 +4361,100 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="70" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="71" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="72" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
+      <c r="J6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="3" t="s">
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" s="2" customFormat="1">
-      <c r="A6" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="2" customFormat="1">
-      <c r="A7" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>14</v>
@@ -4324,30 +4463,27 @@
         <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
@@ -4356,10 +4492,13 @@
         <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>213</v>
+        <v>17</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>19</v>
@@ -4368,30 +4507,27 @@
         <v>20</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="2" customFormat="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>63</v>
+        <v>204</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>19</v>
@@ -4400,51 +4536,57 @@
         <v>20</v>
       </c>
       <c r="L10" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="2" customFormat="1">
-      <c r="A11" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="20"/>
-      <c r="L11" s="21"/>
-    </row>
-    <row r="12" spans="1:14" s="2" customFormat="1">
-      <c r="A12" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>33</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="19" t="s">
-        <v>246</v>
+        <v>65</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -4452,47 +4594,43 @@
       <c r="J12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="19" t="s">
-        <v>73</v>
-      </c>
+      <c r="K12" s="20"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1">
-      <c r="A13" s="22" t="s">
-        <v>216</v>
+    <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>206</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>14</v>
+        <v>218</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>16</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E13" s="21"/>
       <c r="F13" s="19" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
       <c r="J13" s="19" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>188</v>
+        <v>70</v>
       </c>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1">
+    <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>14</v>
@@ -4501,10 +4639,10 @@
         <v>15</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>191</v>
+        <v>235</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -4513,128 +4651,128 @@
         <v>19</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="L15" s="21"/>
+    </row>
+    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="19" t="s">
         <v>217</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" s="2" customFormat="1">
-      <c r="A16" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" s="2" customFormat="1">
-      <c r="A17" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="L17" s="21"/>
-    </row>
-    <row r="18" spans="1:14" s="2" customFormat="1">
-      <c r="A18" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>250</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
       <c r="J18" s="19" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>188</v>
+        <v>70</v>
       </c>
       <c r="L18" s="21"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1">
+    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>14</v>
@@ -4643,10 +4781,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>204</v>
+        <v>240</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -4655,66 +4793,96 @@
         <v>19</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L19" s="21"/>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1">
-      <c r="A20" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="4" t="s">
+    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="C20" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="L20" s="21"/>
+    </row>
+    <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" s="4" customFormat="1" ht="14">
-      <c r="A21" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="F21" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="38" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="17" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="29" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="38" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4727,49 +4895,53 @@
     <hyperlink ref="L3" r:id="rId4" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.6&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{2452B92A-BCEC-455A-85EA-D83C1CF2EB33}"/>
     <hyperlink ref="E4" r:id="rId5" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{B96937E1-79DA-4D39-9804-2E5087DCD349}"/>
     <hyperlink ref="L4" r:id="rId6" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.287&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{2C7C125A-656C-4306-9632-3709E6CACA24}"/>
-    <hyperlink ref="A5" tooltip="Collapse" display=" Geslachtsnaam" xr:uid="{AC2F43A7-337B-4933-8AC8-97703801C3A3}"/>
-    <hyperlink ref="E5" r:id="rId7" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{82D23DA9-F95C-4E21-9299-59A0876B25DB}"/>
-    <hyperlink ref="L5" r:id="rId8" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.291&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{AD7C9E9F-FA09-4623-85FE-BCF1AF995CB2}"/>
-    <hyperlink ref="E6" r:id="rId9" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{C02E8C90-CDCA-4687-B183-A7AA0971F92F}"/>
-    <hyperlink ref="L6" r:id="rId10" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.292&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{199A8CA5-4617-405B-8BB8-C7DE62845322}"/>
-    <hyperlink ref="E7" r:id="rId11" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{CD01B88F-17BB-4C8A-AD14-95E59EC8AD3F}"/>
-    <hyperlink ref="L7" r:id="rId12" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.293&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A488EFD2-3294-4CE8-9425-F3F636ED47EC}"/>
-    <hyperlink ref="E8" r:id="rId13" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{D9479715-D52E-434C-A0D2-740A841E9825}"/>
-    <hyperlink ref="L8" r:id="rId14" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D457B48A-F87F-4BBF-98C9-DE8C19C521DF}"/>
-    <hyperlink ref="E9" r:id="rId15" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{B1517308-039C-498A-A509-B1898CD25CE9}"/>
-    <hyperlink ref="L9" r:id="rId16" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.10&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{99B8DB71-8984-4BD9-80FD-19C98B8E384E}"/>
-    <hyperlink ref="E10" r:id="rId17" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{CB42A5AD-8D6F-4D69-9EB5-C06A9ECA1A23}"/>
-    <hyperlink ref="I10" r:id="rId18" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.0.1.1&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{1543A09C-5DFD-4824-94AA-96C065E3E2DE}"/>
-    <hyperlink ref="L10" r:id="rId19" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.9&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{9EED958F-8E5D-403F-AEE0-0DFD6C968F93}"/>
-    <hyperlink ref="A11" tooltip="Collapse" display=" Onderzoek" xr:uid="{48F6135B-2BF2-4BF7-AAC7-EA8A7DEFFD53}"/>
-    <hyperlink ref="E11" r:id="rId20" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{A886B417-8A7D-445F-9E03-8D1874305B54}"/>
-    <hyperlink ref="L11" r:id="rId21" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{1BFE3189-7962-4A46-A4A6-B827A7AF72B0}"/>
-    <hyperlink ref="A12" tooltip="Collapse" display=" Beeldinformatie" xr:uid="{55610959-22A2-42FD-A4F8-9896F9475954}"/>
-    <hyperlink ref="E12" r:id="rId22" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{47DCC910-2202-4392-B57B-9076592B051B}"/>
-    <hyperlink ref="L12" r:id="rId23" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0A82CADE-8287-4476-BCE5-B94C9CF7B189}"/>
-    <hyperlink ref="E13" r:id="rId24" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{5092114C-2079-43D8-B028-05E846518BC7}"/>
-    <hyperlink ref="L13" r:id="rId25" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{6E677FE2-E514-430C-B482-B497FBC5E86A}"/>
-    <hyperlink ref="E14" r:id="rId26" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{5036A0B5-1CE6-4260-ACA6-F224334E3B8B}"/>
-    <hyperlink ref="L14" r:id="rId27" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{F8A87853-AEAD-4EE4-B510-AB863771B960}"/>
-    <hyperlink ref="E17" r:id="rId28" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{6F497D10-098A-42C6-9606-BEC8703DF0E0}"/>
-    <hyperlink ref="L17" r:id="rId29" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8906220F-44DC-4444-B464-C8166EA3CC46}"/>
-    <hyperlink ref="E18" r:id="rId30" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{72F05734-7A49-49B1-86A5-A9B006BC38C2}"/>
-    <hyperlink ref="L18" r:id="rId31" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{7178A5DE-CA33-4DD7-A9FB-6A00F4D29A19}"/>
-    <hyperlink ref="E19" r:id="rId32" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{6A597C87-C0C3-43D3-9DD4-BB3AA084FCB8}"/>
-    <hyperlink ref="L19" r:id="rId33" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{BAFD298D-553D-4C7D-8A74-98B019F66BC2}"/>
-    <hyperlink ref="A17" tooltip="Collapse" display="Verslaginformatie" xr:uid="{3E168F7D-3021-4E0B-9B8C-8266575D5D1E}"/>
+    <hyperlink ref="A6" tooltip="Collapse" display=" Geslachtsnaam" xr:uid="{AC2F43A7-337B-4933-8AC8-97703801C3A3}"/>
+    <hyperlink ref="E6" r:id="rId7" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{82D23DA9-F95C-4E21-9299-59A0876B25DB}"/>
+    <hyperlink ref="L6" r:id="rId8" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.291&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{AD7C9E9F-FA09-4623-85FE-BCF1AF995CB2}"/>
+    <hyperlink ref="E7" r:id="rId9" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{C02E8C90-CDCA-4687-B183-A7AA0971F92F}"/>
+    <hyperlink ref="L7" r:id="rId10" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.292&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{199A8CA5-4617-405B-8BB8-C7DE62845322}"/>
+    <hyperlink ref="E8" r:id="rId11" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{CD01B88F-17BB-4C8A-AD14-95E59EC8AD3F}"/>
+    <hyperlink ref="L8" r:id="rId12" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.293&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A488EFD2-3294-4CE8-9425-F3F636ED47EC}"/>
+    <hyperlink ref="E9" r:id="rId13" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{D9479715-D52E-434C-A0D2-740A841E9825}"/>
+    <hyperlink ref="L9" r:id="rId14" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D457B48A-F87F-4BBF-98C9-DE8C19C521DF}"/>
+    <hyperlink ref="E10" r:id="rId15" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{B1517308-039C-498A-A509-B1898CD25CE9}"/>
+    <hyperlink ref="L10" r:id="rId16" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.10&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{99B8DB71-8984-4BD9-80FD-19C98B8E384E}"/>
+    <hyperlink ref="E11" r:id="rId17" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{CB42A5AD-8D6F-4D69-9EB5-C06A9ECA1A23}"/>
+    <hyperlink ref="I11" r:id="rId18" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.0.1.1&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{1543A09C-5DFD-4824-94AA-96C065E3E2DE}"/>
+    <hyperlink ref="L11" r:id="rId19" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.9&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{9EED958F-8E5D-403F-AEE0-0DFD6C968F93}"/>
+    <hyperlink ref="A12" tooltip="Collapse" display=" Onderzoek" xr:uid="{48F6135B-2BF2-4BF7-AAC7-EA8A7DEFFD53}"/>
+    <hyperlink ref="E12" r:id="rId20" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{A886B417-8A7D-445F-9E03-8D1874305B54}"/>
+    <hyperlink ref="L12" r:id="rId21" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{1BFE3189-7962-4A46-A4A6-B827A7AF72B0}"/>
+    <hyperlink ref="A13" tooltip="Collapse" display=" Beeldinformatie" xr:uid="{55610959-22A2-42FD-A4F8-9896F9475954}"/>
+    <hyperlink ref="E13" r:id="rId22" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{47DCC910-2202-4392-B57B-9076592B051B}"/>
+    <hyperlink ref="L13" r:id="rId23" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0A82CADE-8287-4476-BCE5-B94C9CF7B189}"/>
+    <hyperlink ref="E14" r:id="rId24" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{5092114C-2079-43D8-B028-05E846518BC7}"/>
+    <hyperlink ref="L14" r:id="rId25" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{6E677FE2-E514-430C-B482-B497FBC5E86A}"/>
+    <hyperlink ref="E15" r:id="rId26" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{5036A0B5-1CE6-4260-ACA6-F224334E3B8B}"/>
+    <hyperlink ref="L15" r:id="rId27" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{F8A87853-AEAD-4EE4-B510-AB863771B960}"/>
+    <hyperlink ref="E18" r:id="rId28" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{6F497D10-098A-42C6-9606-BEC8703DF0E0}"/>
+    <hyperlink ref="L18" r:id="rId29" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8906220F-44DC-4444-B464-C8166EA3CC46}"/>
+    <hyperlink ref="E19" r:id="rId30" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{72F05734-7A49-49B1-86A5-A9B006BC38C2}"/>
+    <hyperlink ref="L19" r:id="rId31" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{7178A5DE-CA33-4DD7-A9FB-6A00F4D29A19}"/>
+    <hyperlink ref="E20" r:id="rId32" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{6A597C87-C0C3-43D3-9DD4-BB3AA084FCB8}"/>
+    <hyperlink ref="L20" r:id="rId33" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{BAFD298D-553D-4C7D-8A74-98B019F66BC2}"/>
+    <hyperlink ref="A18" tooltip="Collapse" display="Verslaginformatie" xr:uid="{3E168F7D-3021-4E0B-9B8C-8266575D5D1E}"/>
+    <hyperlink ref="E5" r:id="rId34" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{6866A7BA-3A75-7E4E-96DF-81DBF6059EE6}"/>
+    <hyperlink ref="L5" r:id="rId35" xr:uid="{9DFF5A40-852E-764D-B8D9-545AD5BBCDEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5002,20 +5174,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5040,12 +5213,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DOSINZAGE2-701: Extended Modality value set, updated profile and IG
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D605F28-540E-A64C-BC82-6179099E6EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1318A171-03B4-764F-BC17-8F5BE6571FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="29080" windowHeight="16400" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19060" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
   <sheets>
     <sheet name="Beeld en verslag tijdlijn raadp" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="278">
   <si>
     <t>Naam</t>
   </si>
@@ -806,9 +806,6 @@
     <t>Het medische beeldvormingsapparaat, zoals een CT-scanner of een MRI-machine, dat wordt gebruikt om de beelden te verkrijgen.</t>
   </si>
   <si>
-    <t>Modalities</t>
-  </si>
-  <si>
     <t>2.4.1 AccessionNumber</t>
   </si>
   <si>
@@ -877,13 +874,19 @@
   </si>
   <si>
     <t>0 … *</t>
+  </si>
+  <si>
+    <t>Modalities*</t>
+  </si>
+  <si>
+    <t>*OT en SC zijn toegevoegd aan de waardelijst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1433,10 +1436,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1797,7 +1800,7 @@
       <selection activeCell="G1" activeCellId="1" sqref="F1:F1048576 G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="5" width="11" customWidth="1"/>
@@ -1805,7 +1808,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>12</v>
       </c>
@@ -1856,7 +1859,7 @@
       <c r="D2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="66" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="64" t="s">
@@ -1865,39 +1868,34 @@
       <c r="G2" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
       <c r="J2" s="64" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="68" t="s">
+      <c r="L2" s="66" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="65"/>
       <c r="B3" s="65"/>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
-      <c r="E3" s="69"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="65"/>
       <c r="G3" s="65"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
       <c r="J3" s="65"/>
       <c r="K3" s="65"/>
-      <c r="L3" s="69"/>
+      <c r="L3" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1905,6 +1903,11 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1918,11 +1921,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" style="55" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="37" customWidth="1"/>
@@ -1930,11 +1933,14 @@
     <col min="5" max="5" width="11" style="37" customWidth="1"/>
     <col min="6" max="6" width="105.6640625" style="63" customWidth="1"/>
     <col min="7" max="7" width="44" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="241" width="11" style="37" customWidth="1"/>
+    <col min="8" max="10" width="11" style="37" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.33203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="241" width="11" style="37" customWidth="1"/>
     <col min="242" max="16384" width="8.83203125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1">
+    <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +1978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="34" customFormat="1">
+    <row r="2" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="10" customFormat="1">
+    <row r="3" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>27</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1">
+    <row r="4" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>31</v>
       </c>
@@ -2055,7 +2061,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1">
+    <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
         <v>38</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1">
+    <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>42</v>
       </c>
@@ -2117,7 +2123,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1">
+    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>47</v>
       </c>
@@ -2149,7 +2155,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>51</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1">
+    <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="45" t="s">
         <v>53</v>
       </c>
@@ -2213,7 +2219,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="10" customFormat="1">
+    <row r="10" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
         <v>59</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="10" customFormat="1">
+    <row r="11" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
         <v>65</v>
       </c>
@@ -2273,7 +2279,7 @@
       <c r="K11" s="34"/>
       <c r="L11" s="33"/>
     </row>
-    <row r="12" spans="1:15" s="10" customFormat="1">
+    <row r="12" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="47" t="s">
         <v>69</v>
       </c>
@@ -2303,7 +2309,7 @@
       </c>
       <c r="L12" s="33"/>
     </row>
-    <row r="13" spans="1:15" s="10" customFormat="1">
+    <row r="13" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
         <v>74</v>
       </c>
@@ -2333,7 +2339,7 @@
       </c>
       <c r="L13" s="33"/>
     </row>
-    <row r="14" spans="1:15" s="10" customFormat="1">
+    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
         <v>78</v>
       </c>
@@ -2365,7 +2371,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="10" customFormat="1" ht="105">
+    <row r="15" spans="1:15" s="10" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A15" s="42" t="s">
         <v>82</v>
       </c>
@@ -2400,7 +2406,7 @@
       <c r="N15" s="35"/>
       <c r="O15" s="35"/>
     </row>
-    <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1">
+    <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="43" t="s">
         <v>85</v>
       </c>
@@ -2430,7 +2436,7 @@
       </c>
       <c r="L16" s="33"/>
     </row>
-    <row r="17" spans="1:12" s="34" customFormat="1">
+    <row r="17" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="48" t="s">
         <v>88</v>
       </c>
@@ -2463,7 +2469,7 @@
       </c>
       <c r="L17" s="33"/>
     </row>
-    <row r="18" spans="1:12" s="10" customFormat="1">
+    <row r="18" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="49" t="s">
         <v>94</v>
       </c>
@@ -2482,10 +2488,16 @@
       <c r="F18" s="60" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1">
+      <c r="J18" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>97</v>
@@ -2513,9 +2525,9 @@
       </c>
       <c r="L19" s="33"/>
     </row>
-    <row r="20" spans="1:12" s="10" customFormat="1">
+    <row r="20" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="51" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>100</v>
@@ -2543,7 +2555,7 @@
       </c>
       <c r="L20" s="33"/>
     </row>
-    <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="42" t="s">
         <v>103</v>
       </c>
@@ -2575,7 +2587,7 @@
       </c>
       <c r="L21" s="33"/>
     </row>
-    <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+    <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="42" t="s">
         <v>108</v>
       </c>
@@ -2607,7 +2619,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="10" customFormat="1">
+    <row r="23" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="42" t="s">
         <v>112</v>
       </c>
@@ -2639,7 +2651,7 @@
       </c>
       <c r="L23" s="33"/>
     </row>
-    <row r="24" spans="1:12" s="10" customFormat="1">
+    <row r="24" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49" t="s">
         <v>116</v>
       </c>
@@ -2671,7 +2683,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="10" customFormat="1">
+    <row r="25" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="43" t="s">
         <v>121</v>
       </c>
@@ -2699,7 +2711,7 @@
       </c>
       <c r="L25" s="33"/>
     </row>
-    <row r="26" spans="1:12" s="10" customFormat="1">
+    <row r="26" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="50" t="s">
         <v>124</v>
       </c>
@@ -2729,7 +2741,7 @@
       </c>
       <c r="L26" s="33"/>
     </row>
-    <row r="27" spans="1:12" s="10" customFormat="1">
+    <row r="27" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="42" t="s">
         <v>129</v>
       </c>
@@ -2761,7 +2773,7 @@
       </c>
       <c r="L27" s="33"/>
     </row>
-    <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1">
+    <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43" t="s">
         <v>134</v>
       </c>
@@ -2791,7 +2803,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="10" customFormat="1">
+    <row r="29" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
@@ -2823,7 +2835,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="10" customFormat="1">
+    <row r="30" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="43" t="s">
         <v>142</v>
       </c>
@@ -2853,7 +2865,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="10" customFormat="1">
+    <row r="31" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="42" t="s">
         <v>145</v>
       </c>
@@ -2885,7 +2897,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="10" customFormat="1">
+    <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="42" t="s">
         <v>149</v>
       </c>
@@ -2917,7 +2929,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="10" customFormat="1">
+    <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="42" t="s">
         <v>153</v>
       </c>
@@ -2951,7 +2963,7 @@
       </c>
       <c r="L33" s="33"/>
     </row>
-    <row r="34" spans="1:12" s="34" customFormat="1" ht="45">
+    <row r="34" spans="1:13" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" s="43" t="s">
         <v>158</v>
       </c>
@@ -2962,11 +2974,11 @@
         <v>14</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E34" s="33"/>
       <c r="F34" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J34" s="32" t="s">
         <v>25</v>
@@ -2976,7 +2988,7 @@
       </c>
       <c r="L34" s="33"/>
     </row>
-    <row r="35" spans="1:12" s="10" customFormat="1">
+    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="50" t="s">
         <v>160</v>
       </c>
@@ -3004,7 +3016,7 @@
       </c>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" s="10" customFormat="1">
+    <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="42" t="s">
         <v>163</v>
       </c>
@@ -3036,7 +3048,7 @@
       </c>
       <c r="L36" s="33"/>
     </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+    <row r="37" spans="1:13" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="43" t="s">
         <v>165</v>
       </c>
@@ -3066,7 +3078,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="10" customFormat="1">
+    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="42" t="s">
         <v>167</v>
       </c>
@@ -3098,7 +3110,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="10" customFormat="1">
+    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="43" t="s">
         <v>169</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="10" customFormat="1">
+    <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="42" t="s">
         <v>171</v>
       </c>
@@ -3160,7 +3172,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="10" customFormat="1">
+    <row r="41" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="42" t="s">
         <v>173</v>
       </c>
@@ -3192,7 +3204,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="10" customFormat="1">
+    <row r="42" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="42" t="s">
         <v>175</v>
       </c>
@@ -3226,7 +3238,7 @@
       </c>
       <c r="L42" s="33"/>
     </row>
-    <row r="43" spans="1:12" s="10" customFormat="1">
+    <row r="43" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="42" t="s">
         <v>177</v>
       </c>
@@ -3260,7 +3272,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="10" customFormat="1">
+    <row r="44" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="52" t="s">
         <v>183</v>
       </c>
@@ -3288,7 +3300,7 @@
       </c>
       <c r="L44" s="33"/>
     </row>
-    <row r="45" spans="1:12" s="10" customFormat="1">
+    <row r="45" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="42" t="s">
         <v>185</v>
       </c>
@@ -3318,7 +3330,7 @@
       </c>
       <c r="L45" s="33"/>
     </row>
-    <row r="46" spans="1:12" s="10" customFormat="1">
+    <row r="46" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="42" t="s">
         <v>189</v>
       </c>
@@ -3348,7 +3360,7 @@
       </c>
       <c r="L46" s="33"/>
     </row>
-    <row r="47" spans="1:12" s="10" customFormat="1">
+    <row r="47" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="49" t="s">
         <v>192</v>
       </c>
@@ -3376,7 +3388,7 @@
       </c>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" s="10" customFormat="1">
+    <row r="48" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="53" t="s">
         <v>240</v>
       </c>
@@ -3398,7 +3410,7 @@
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
       <c r="I48" s="33" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="J48" s="32" t="s">
         <v>19</v>
@@ -3407,8 +3419,11 @@
         <v>188</v>
       </c>
       <c r="L48" s="33"/>
-    </row>
-    <row r="49" spans="1:12" s="10" customFormat="1">
+      <c r="M48" s="10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="52" t="s">
         <v>197</v>
       </c>
@@ -3436,7 +3451,7 @@
       </c>
       <c r="L49" s="33"/>
     </row>
-    <row r="50" spans="1:12" s="10" customFormat="1">
+    <row r="50" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="42" t="s">
         <v>199</v>
       </c>
@@ -3466,7 +3481,7 @@
       </c>
       <c r="L50" s="33"/>
     </row>
-    <row r="51" spans="1:12" s="10" customFormat="1">
+    <row r="51" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="42" t="s">
         <v>202</v>
       </c>
@@ -3496,7 +3511,7 @@
       </c>
       <c r="L51" s="33"/>
     </row>
-    <row r="52" spans="1:12" s="10" customFormat="1">
+    <row r="52" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="49" t="s">
         <v>205</v>
       </c>
@@ -3524,21 +3539,21 @@
       </c>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="1:12" s="50" customFormat="1" ht="15">
+    <row r="53" spans="1:12" s="50" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="54" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C53" s="50" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="F53" s="62" t="s">
         <v>260</v>
-      </c>
-      <c r="F53" s="62" t="s">
-        <v>261</v>
       </c>
       <c r="G53" s="57"/>
       <c r="H53" s="57"/>
@@ -3551,9 +3566,9 @@
       </c>
       <c r="L53" s="58"/>
     </row>
-    <row r="54" spans="1:12" s="10" customFormat="1">
+    <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="53" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B54" s="32" t="s">
         <v>232</v>
@@ -3562,7 +3577,7 @@
         <v>14</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E54" s="33" t="s">
         <v>16</v>
@@ -3577,26 +3592,26 @@
         <v>19</v>
       </c>
       <c r="K54" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L54" s="33"/>
     </row>
-    <row r="55" spans="1:12" s="10" customFormat="1">
+    <row r="55" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="53" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C55" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E55" s="33"/>
       <c r="F55" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G55" s="34"/>
       <c r="H55" s="34"/>
@@ -3605,22 +3620,22 @@
         <v>19</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L55" s="33"/>
     </row>
-    <row r="56" spans="1:12" s="10" customFormat="1">
+    <row r="56" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="51" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C56" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E56" s="33"/>
       <c r="F56" s="30" t="s">
@@ -3639,18 +3654,18 @@
       </c>
       <c r="L56" s="33"/>
     </row>
-    <row r="57" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="57" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C57" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E57" s="33" t="s">
         <v>16</v>
@@ -3671,12 +3686,12 @@
       </c>
       <c r="L57" s="33"/>
     </row>
-    <row r="58" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+    <row r="58" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C58" s="32" t="s">
         <v>14</v>
@@ -3703,12 +3718,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="10" customFormat="1">
+    <row r="59" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="42" t="s">
         <v>112</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C59" s="32" t="s">
         <v>14</v>
@@ -3735,12 +3750,12 @@
       </c>
       <c r="L59" s="33"/>
     </row>
-    <row r="60" spans="1:12" s="10" customFormat="1">
+    <row r="60" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>14</v>
@@ -3767,7 +3782,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="10" customFormat="1">
+    <row r="61" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="54" t="s">
         <v>234</v>
       </c>
@@ -3917,7 +3932,7 @@
     <hyperlink ref="E54" r:id="rId114" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{06898B6A-A0ED-0244-9A16-72B56DEBED42}"/>
     <hyperlink ref="E61" r:id="rId115" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{EABED256-857D-2642-BE3E-5AD20C03336E}"/>
     <hyperlink ref="E48" r:id="rId116" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{0BB16F56-88D4-5644-B710-8B7860CB1712}"/>
-    <hyperlink ref="I48" r:id="rId117" xr:uid="{E48A8B75-06B7-5444-866E-89BA6FC9A9FC}"/>
+    <hyperlink ref="I48" r:id="rId117" display="Modalities" xr:uid="{E48A8B75-06B7-5444-866E-89BA6FC9A9FC}"/>
     <hyperlink ref="E56" r:id="rId118" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{24C31C8F-A2E9-824A-9317-3AA15CB5B012}"/>
     <hyperlink ref="H56" r:id="rId119" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{C869B80E-2110-5741-BB09-F7EDBF5A7FAE}"/>
     <hyperlink ref="L56" r:id="rId120" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D915B272-925A-FB46-A898-7CF03503B973}"/>
@@ -3944,13 +3959,13 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3988,7 +4003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -4021,7 +4036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>209</v>
       </c>
@@ -4049,7 +4064,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1">
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>210</v>
       </c>
@@ -4098,7 +4113,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="17" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -4107,7 +4122,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4145,7 +4160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>211</v>
       </c>
@@ -4169,7 +4184,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1">
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>27</v>
       </c>
@@ -4196,7 +4211,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1">
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -4225,7 +4240,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1">
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>38</v>
       </c>
@@ -4252,7 +4267,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1">
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -4281,7 +4296,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1">
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
@@ -4310,7 +4325,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>51</v>
       </c>
@@ -4342,7 +4357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="9" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>53</v>
       </c>
@@ -4371,7 +4386,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="2" customFormat="1">
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>59</v>
       </c>
@@ -4403,7 +4418,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1">
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>65</v>
       </c>
@@ -4429,7 +4444,7 @@
       <c r="K11" s="20"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1">
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>215</v>
       </c>
@@ -4457,7 +4472,7 @@
       </c>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1">
+    <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>216</v>
       </c>
@@ -4487,7 +4502,7 @@
       </c>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1">
+    <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>239</v>
       </c>
@@ -4517,7 +4532,7 @@
       </c>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1">
+    <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>217</v>
       </c>
@@ -4547,7 +4562,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1">
+    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>218</v>
       </c>
@@ -4571,7 +4586,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1">
+    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>220</v>
       </c>
@@ -4599,7 +4614,7 @@
       </c>
       <c r="L17" s="21"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1">
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>221</v>
       </c>
@@ -4629,7 +4644,7 @@
       </c>
       <c r="L18" s="21"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1">
+    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>222</v>
       </c>
@@ -4659,7 +4674,7 @@
       </c>
       <c r="L19" s="21"/>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1">
+    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>224</v>
       </c>
@@ -4689,7 +4704,7 @@
       <c r="M20" s="4"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" s="4" customFormat="1" ht="14">
+    <row r="21" spans="1:14" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>225</v>
       </c>
@@ -4707,12 +4722,12 @@
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="29" t="s">
         <v>229</v>
       </c>
@@ -4764,12 +4779,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5002,20 +5019,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5040,12 +5058,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DOSINZAGE2-586: Removed the concept Requester
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88408938-5D5F-4445-B1C3-4B76435670B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E59351-303B-654C-9872-AFDE7F20F298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38540" yWindow="660" windowWidth="38080" windowHeight="20800" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
+    <workbookView xWindow="140" yWindow="660" windowWidth="38080" windowHeight="19380" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
   <sheets>
     <sheet name="Beeld en verslag tijdlijn raadp" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name=" Beeld &amp;Verslag beschikbaar" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Beeld en verslag tijdlijn besch'!$A$1:$N$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Beeld en verslag tijdlijn besch'!$A$1:$N$45</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="265">
   <si>
     <t>Naam</t>
   </si>
@@ -398,36 +398,18 @@
     <t>NL-CM-17.2.4</t>
   </si>
   <si>
-    <t> 2.1.6.Aanvrager</t>
-  </si>
-  <si>
-    <t>bbs-dataelement-189</t>
-  </si>
-  <si>
-    <t>De zorgverlener die de verrichting heeft aangevraagd. In de meeste gevallen wordt alleen het specialisme en niet de naam van de zorgverlener doorgegeven.</t>
-  </si>
-  <si>
     <t> 2.1.6.1.Zorgverlener</t>
   </si>
   <si>
-    <t>bbs-dataelement-423</t>
-  </si>
-  <si>
     <t>Rootconcept van de bouwsteen Zorgverlener. Dit rootconcept bevat alle gegevenselementen van de bouwsteen Zorgverlener.</t>
   </si>
   <si>
     <t>gezondheidszorgpersoneel (SNOMED Clinical Terms: 223366009)</t>
   </si>
   <si>
-    <t>Aanvrager</t>
-  </si>
-  <si>
     <t> 2.1.6.1.1. ZorgverlenerIdentificatienummer</t>
   </si>
   <si>
-    <t>bbs-dataelement-424</t>
-  </si>
-  <si>
     <t>Het zorgverleneridentificatienummer is een nummer dat de zorgverlener uniek identificeert.</t>
   </si>
   <si>
@@ -437,12 +419,6 @@
     <t>Zorgverlener</t>
   </si>
   <si>
-    <t>  2.1.6.1.2.Naamgegevens</t>
-  </si>
-  <si>
-    <t>bbs-dataelement-425</t>
-  </si>
-  <si>
     <t>De naamgegevens van de zorgverlener. Indien een zorgverleneridentificatienummer wordt opgegeven, is dit de naam zoals vermeld in UZI, AGB of in de instelling.</t>
   </si>
   <si>
@@ -452,33 +428,21 @@
     <t> 2.1.6.1.2.1. Voornamen</t>
   </si>
   <si>
-    <t>bbs-dataelement-426</t>
-  </si>
-  <si>
     <t>Voornamen van de zorgverlener</t>
   </si>
   <si>
     <t>zib2020bbr-dataelementen-496</t>
   </si>
   <si>
-    <t>bbs-dataelement-430</t>
-  </si>
-  <si>
     <t>zib2020bbr-dataelementen-500</t>
   </si>
   <si>
-    <t>bbs-dataelement-431</t>
-  </si>
-  <si>
     <t>Voorvoegsel van de achternaam van de zorgverlener</t>
   </si>
   <si>
     <t>zib2020bbr-dataelementen-501</t>
   </si>
   <si>
-    <t>bbs-dataelement-432</t>
-  </si>
-  <si>
     <t>Achternaam van de zorgverlener</t>
   </si>
   <si>
@@ -488,9 +452,6 @@
     <t>  2.1.6.1.3. Specialisme</t>
   </si>
   <si>
-    <t>bbs-dataelement-437</t>
-  </si>
-  <si>
     <t xml:space="preserve">Medisch specialisme van de zorgverlener. </t>
   </si>
   <si>
@@ -500,36 +461,21 @@
     <t>SpecialismeUZICodelijst 2020-09-01T00:00:00 (statisch / Verplicht/CNE)</t>
   </si>
   <si>
-    <t> 2.1.7.Uitvoerder</t>
-  </si>
-  <si>
     <t>bbs-dataelement-187</t>
   </si>
   <si>
-    <t> 2.1.7.1.Zorgverlener</t>
-  </si>
-  <si>
     <t>bbs-dataelement-383</t>
   </si>
   <si>
     <t>Uitvoerder</t>
   </si>
   <si>
-    <t> 2.1.7.1.1. ZorgverlenerIdentificatienummer</t>
-  </si>
-  <si>
     <t>bbs-dataelement-384</t>
   </si>
   <si>
-    <t> 2 .1.7.1.2.Naamgegevens</t>
-  </si>
-  <si>
     <t>bbs-dataelement-385</t>
   </si>
   <si>
-    <t> 2.1.7.1.2.1. Voornamen</t>
-  </si>
-  <si>
     <t>bbs-dataelement-386</t>
   </si>
   <si>
@@ -542,13 +488,7 @@
     <t>bbs-dataelement-392</t>
   </si>
   <si>
-    <t>  2.1.7.1.3. Specialisme</t>
-  </si>
-  <si>
     <t>bbs-dataelement-397</t>
-  </si>
-  <si>
-    <t>  2.1.7.1.4. ZorgverlenerRol</t>
   </si>
   <si>
     <t>bbs-dataelement-422</t>
@@ -870,33 +810,15 @@
     <t> 2.1.6.1.2.3.1. Voorvoegsels</t>
   </si>
   <si>
-    <t> 2.1.6.1.2.3.1. Achternaam</t>
-  </si>
-  <si>
     <t> 2.1.6.1.2.3. Geslachtsnaam</t>
   </si>
   <si>
-    <t>bbs-dataelement-427</t>
-  </si>
-  <si>
     <t>zib2020bbr-dataelementen-497</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2.1.7.1.2.2. Initialen</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2.1.6.1.2.2. Initialen</t>
   </si>
   <si>
-    <t> 2.1.7.1.2.3. Geslachtsnaam</t>
-  </si>
-  <si>
-    <t> 2.1.7.1.2.3.1. Voorvoegsels</t>
-  </si>
-  <si>
-    <t> 2.1.7.1.2.3.2. Achternaam</t>
-  </si>
-  <si>
     <t>bbs-dataelement-387</t>
   </si>
   <si>
@@ -907,6 +829,18 @@
   </si>
   <si>
     <t>Modalities*</t>
+  </si>
+  <si>
+    <t> 2.1.6.Uitvoerder</t>
+  </si>
+  <si>
+    <t> 2 .1.6.1.2.Naamgegevens</t>
+  </si>
+  <si>
+    <t> 2.1.6.1.2.3.2. Achternaam</t>
+  </si>
+  <si>
+    <t>  2.1.6.1.4. ZorgverlenerRol</t>
   </si>
 </sst>
 </file>
@@ -1467,10 +1401,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1828,7 +1762,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" activeCellId="1" sqref="F1:F1048576 G1:G1048576"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1890,7 +1824,7 @@
       <c r="D2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="68" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="66" t="s">
@@ -1899,15 +1833,15 @@
       <c r="G2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
       <c r="J2" s="66" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="70" t="s">
+      <c r="L2" s="68" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1916,22 +1850,17 @@
       <c r="B3" s="67"/>
       <c r="C3" s="67"/>
       <c r="D3" s="67"/>
-      <c r="E3" s="71"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="67"/>
       <c r="G3" s="67"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
       <c r="J3" s="67"/>
       <c r="K3" s="67"/>
-      <c r="L3" s="71"/>
+      <c r="L3" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1939,6 +1868,11 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1950,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2094,10 +2028,10 @@
     </row>
     <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>14</v>
@@ -2109,7 +2043,7 @@
         <v>34</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
@@ -2121,12 +2055,12 @@
         <v>36</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>38</v>
@@ -2156,7 +2090,7 @@
     </row>
     <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>41</v>
@@ -2188,7 +2122,7 @@
     </row>
     <row r="8" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>45</v>
@@ -2451,7 +2385,7 @@
         <v>58</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
@@ -2484,7 +2418,7 @@
       </c>
       <c r="E17" s="33"/>
       <c r="F17" s="61" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="G17" s="34"/>
       <c r="H17" s="33" t="s">
@@ -2549,7 +2483,7 @@
         <v>58</v>
       </c>
       <c r="F19" s="60" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="J19" s="32" t="s">
         <v>19</v>
@@ -2560,7 +2494,7 @@
     </row>
     <row r="20" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="50" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>94</v>
@@ -2590,7 +2524,7 @@
     </row>
     <row r="21" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="51" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>97</v>
@@ -2746,26 +2680,23 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
-        <v>118</v>
+        <v>261</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="C26" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>33</v>
+        <v>245</v>
       </c>
       <c r="E26" s="33"/>
-      <c r="F26" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
+      <c r="F26" s="30" t="s">
+        <v>244</v>
+      </c>
       <c r="J26" s="32" t="s">
         <v>25</v>
       </c>
@@ -2776,40 +2707,38 @@
     </row>
     <row r="27" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="33"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="G27" s="34"/>
-      <c r="H27" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J27" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="L27" s="33"/>
+      <c r="K27" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="L27" s="12"/>
     </row>
     <row r="28" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="42" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>14</v>
@@ -2821,10 +2750,10 @@
         <v>16</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
@@ -2832,16 +2761,16 @@
         <v>19</v>
       </c>
       <c r="K28" s="32" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="L28" s="33"/>
     </row>
-    <row r="29" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="43" t="s">
-        <v>131</v>
+        <v>262</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C29" s="32" t="s">
         <v>14</v>
@@ -2851,7 +2780,7 @@
       </c>
       <c r="E29" s="33"/>
       <c r="F29" s="30" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
@@ -2860,18 +2789,18 @@
         <v>25</v>
       </c>
       <c r="K29" s="32" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="L29" s="33" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="42" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C30" s="32" t="s">
         <v>14</v>
@@ -2883,7 +2812,7 @@
         <v>34</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
@@ -2895,15 +2824,15 @@
         <v>36</v>
       </c>
       <c r="L30" s="33" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="C31" s="32" t="s">
         <v>14</v>
@@ -2915,7 +2844,7 @@
         <v>34</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
@@ -2927,15 +2856,15 @@
         <v>36</v>
       </c>
       <c r="L31" s="33" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C32" s="32" t="s">
         <v>14</v>
@@ -2957,15 +2886,15 @@
         <v>36</v>
       </c>
       <c r="L32" s="33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="42" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C33" s="32" t="s">
         <v>14</v>
@@ -2977,7 +2906,7 @@
         <v>34</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
@@ -2989,15 +2918,15 @@
         <v>43</v>
       </c>
       <c r="L33" s="33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="42" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C34" s="32" t="s">
         <v>14</v>
@@ -3009,7 +2938,7 @@
         <v>34</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
@@ -3021,12 +2950,12 @@
         <v>43</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="42" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B35" s="32" t="s">
         <v>148</v>
@@ -3041,82 +2970,91 @@
         <v>58</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="G35" s="34"/>
       <c r="H35" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="J35" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="L35" s="33"/>
+    </row>
+    <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="42" t="s">
+        <v>264</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="I35" s="33" t="s">
+      <c r="E36" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="J35" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K35" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="L35" s="33"/>
-    </row>
-    <row r="36" spans="1:12" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A36" s="43" t="s">
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="J36" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="L36" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="E36" s="33"/>
-      <c r="F36" s="30" t="s">
-        <v>264</v>
-      </c>
-      <c r="J36" s="32" t="s">
+    </row>
+    <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="33"/>
+      <c r="F37" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="K36" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="L36" s="33"/>
-    </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="J37" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K37" s="11" t="s">
+      <c r="K37" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="L37" s="33"/>
+    </row>
+    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="L37" s="12"/>
-    </row>
-    <row r="38" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="42" t="s">
+      <c r="B38" s="32" t="s">
         <v>157</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>158</v>
       </c>
       <c r="C38" s="32" t="s">
         <v>14</v>
@@ -3128,27 +3066,25 @@
         <v>16</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" s="32" t="s">
-        <v>129</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="G38" s="34"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
       <c r="J38" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K38" s="32" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="L38" s="33"/>
     </row>
-    <row r="39" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="43" t="s">
-        <v>159</v>
+    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="42" t="s">
+        <v>160</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C39" s="32" t="s">
         <v>14</v>
@@ -3156,103 +3092,102 @@
       <c r="D39" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="F39" s="30" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
       <c r="J39" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K39" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="L39" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="L39" s="33"/>
+    </row>
+    <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F40" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K40" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="L40" s="33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F40" s="60" t="s">
+        <v>167</v>
+      </c>
+      <c r="I40" s="12"/>
+      <c r="J40" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="L40" s="12"/>
+    </row>
+    <row r="41" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="53" t="s">
-        <v>278</v>
+        <v>211</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>283</v>
+        <v>212</v>
       </c>
       <c r="C41" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>33</v>
+        <v>258</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
+      <c r="I41" s="33" t="s">
+        <v>260</v>
+      </c>
       <c r="J41" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K41" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="L41" s="33" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="43" t="s">
-        <v>280</v>
+        <v>159</v>
+      </c>
+      <c r="L41" s="33"/>
+      <c r="M41" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="52" t="s">
+        <v>168</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C42" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E42" s="33"/>
       <c r="F42" s="30" t="s">
-        <v>39</v>
+        <v>217</v>
       </c>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
@@ -3261,30 +3196,28 @@
         <v>25</v>
       </c>
       <c r="K42" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="L42" s="33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="L42" s="33"/>
+    </row>
+    <row r="43" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="42" t="s">
-        <v>281</v>
+        <v>170</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C43" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
@@ -3293,18 +3226,16 @@
         <v>19</v>
       </c>
       <c r="K43" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="L43" s="33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="L43" s="33"/>
+    </row>
+    <row r="44" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="42" t="s">
-        <v>282</v>
+        <v>173</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C44" s="32" t="s">
         <v>14</v>
@@ -3313,10 +3244,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
@@ -3325,622 +3256,313 @@
         <v>19</v>
       </c>
       <c r="K44" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="L44" s="33" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="42" t="s">
-        <v>166</v>
-      </c>
-      <c r="B45" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="C45" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="F45" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="G45" s="34"/>
-      <c r="H45" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="I45" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="J45" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K45" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="L45" s="33"/>
-    </row>
-    <row r="46" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="42" t="s">
-        <v>168</v>
-      </c>
-      <c r="B46" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C46" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="E46" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="F46" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="J46" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K46" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="L46" s="33" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="52" t="s">
-        <v>174</v>
+      <c r="L44" s="33"/>
+    </row>
+    <row r="45" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="I45" s="12"/>
+      <c r="J45" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="L45" s="12"/>
+    </row>
+    <row r="46" spans="1:13" s="50" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="54" t="s">
+        <v>224</v>
+      </c>
+      <c r="B46" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="C46" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="F46" s="62" t="s">
+        <v>230</v>
+      </c>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="L46" s="58"/>
+    </row>
+    <row r="47" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="53" t="s">
+        <v>223</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="C47" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="33"/>
+      <c r="D47" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E47" s="33" t="s">
+        <v>16</v>
+      </c>
       <c r="F47" s="30" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="G47" s="34"/>
       <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
+      <c r="I47" s="33"/>
       <c r="J47" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K47" s="32" t="s">
-        <v>70</v>
+        <v>19</v>
+      </c>
+      <c r="K47" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="L47" s="33"/>
     </row>
-    <row r="48" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="42" t="s">
-        <v>176</v>
+    <row r="48" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="53" t="s">
+        <v>242</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="C48" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="33" t="s">
-        <v>16</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="E48" s="33"/>
       <c r="F48" s="30" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
+      <c r="I48" s="33"/>
       <c r="J48" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K48" s="32" t="s">
-        <v>179</v>
+      <c r="K48" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="L48" s="33"/>
     </row>
-    <row r="49" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="42" t="s">
-        <v>180</v>
+    <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="51" t="s">
+        <v>239</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>181</v>
+        <v>234</v>
       </c>
       <c r="C49" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="33" t="s">
-        <v>53</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="E49" s="33"/>
       <c r="F49" s="30" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
+      <c r="H49" s="33" t="s">
+        <v>96</v>
+      </c>
       <c r="I49" s="34"/>
       <c r="J49" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K49" s="32" t="s">
-        <v>179</v>
+        <v>99</v>
       </c>
       <c r="L49" s="33"/>
     </row>
-    <row r="50" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="E50" s="12" t="s">
+    <row r="50" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G50" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L50" s="33"/>
+    </row>
+    <row r="51" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="B51" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F50" s="60" t="s">
-        <v>187</v>
-      </c>
-      <c r="I50" s="12"/>
-      <c r="J50" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="L50" s="12"/>
-    </row>
-    <row r="51" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="53" t="s">
-        <v>231</v>
-      </c>
-      <c r="B51" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="C51" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="32" t="s">
-        <v>284</v>
-      </c>
-      <c r="E51" s="33" t="s">
-        <v>58</v>
-      </c>
       <c r="F51" s="30" t="s">
-        <v>242</v>
+        <v>107</v>
       </c>
       <c r="G51" s="34"/>
       <c r="H51" s="34"/>
-      <c r="I51" s="33" t="s">
-        <v>286</v>
-      </c>
+      <c r="I51" s="34"/>
       <c r="J51" s="32" t="s">
         <v>19</v>
       </c>
       <c r="K51" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="L51" s="33"/>
-      <c r="M51" s="10" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="52" t="s">
-        <v>188</v>
+        <v>104</v>
+      </c>
+      <c r="L51" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="42" t="s">
+        <v>109</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>189</v>
+        <v>237</v>
       </c>
       <c r="C52" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" s="33"/>
-      <c r="F52" s="30" t="s">
-        <v>237</v>
+        <v>93</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F52" s="60" t="s">
+        <v>111</v>
       </c>
       <c r="G52" s="34"/>
       <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
+      <c r="I52" s="33" t="s">
+        <v>112</v>
+      </c>
       <c r="J52" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K52" s="32" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="L52" s="33"/>
     </row>
-    <row r="53" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="42" t="s">
-        <v>190</v>
+    <row r="53" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="49" t="s">
+        <v>233</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="C53" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E53" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F53" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="L53" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="30" t="s">
-        <v>234</v>
-      </c>
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K53" s="32" t="s">
-        <v>192</v>
-      </c>
-      <c r="L53" s="33"/>
-    </row>
-    <row r="54" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="42" t="s">
-        <v>193</v>
-      </c>
-      <c r="B54" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="C54" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E54" s="33" t="s">
-        <v>53</v>
-      </c>
       <c r="F54" s="30" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="G54" s="34"/>
       <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
+      <c r="I54" s="33"/>
       <c r="J54" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="K54" s="32" t="s">
-        <v>192</v>
+      <c r="K54" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="L54" s="33"/>
     </row>
-    <row r="55" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F55" s="60" t="s">
-        <v>233</v>
-      </c>
-      <c r="I55" s="12"/>
-      <c r="J55" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K55" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="L55" s="12"/>
-    </row>
-    <row r="56" spans="1:13" s="50" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="54" t="s">
-        <v>244</v>
-      </c>
-      <c r="B56" s="50" t="s">
-        <v>246</v>
-      </c>
-      <c r="C56" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="50" t="s">
-        <v>249</v>
-      </c>
-      <c r="F56" s="62" t="s">
-        <v>250</v>
-      </c>
-      <c r="G56" s="57"/>
-      <c r="H56" s="57"/>
-      <c r="I56" s="58"/>
-      <c r="J56" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="K56" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="L56" s="58"/>
-    </row>
-    <row r="57" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="53" t="s">
-        <v>243</v>
-      </c>
-      <c r="B57" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="C57" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="E57" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F57" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="G57" s="34"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K57" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="L57" s="33"/>
-    </row>
-    <row r="58" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="B58" s="32" t="s">
-        <v>248</v>
-      </c>
-      <c r="C58" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="E58" s="33"/>
-      <c r="F58" s="30" t="s">
-        <v>263</v>
-      </c>
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K58" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="L58" s="33"/>
-    </row>
-    <row r="59" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="51" t="s">
-        <v>259</v>
-      </c>
-      <c r="B59" s="32" t="s">
-        <v>254</v>
-      </c>
-      <c r="C59" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="E59" s="33"/>
-      <c r="F59" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="G59" s="34"/>
-      <c r="H59" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="I59" s="34"/>
-      <c r="J59" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K59" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="L59" s="33"/>
-    </row>
-    <row r="60" spans="1:13" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="B60" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="C60" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="E60" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F60" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="G60" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K60" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="L60" s="33"/>
-    </row>
-    <row r="61" spans="1:13" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="B61" s="32" t="s">
-        <v>256</v>
-      </c>
-      <c r="C61" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E61" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F61" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="G61" s="34"/>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K61" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="L61" s="33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="B62" s="32" t="s">
-        <v>257</v>
-      </c>
-      <c r="C62" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D62" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E62" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="F62" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="G62" s="34"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="J62" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K62" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="L62" s="33"/>
-    </row>
-    <row r="63" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="B63" s="32" t="s">
-        <v>258</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F63" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="I63" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="J63" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K63" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L63" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="54" t="s">
-        <v>225</v>
-      </c>
-      <c r="B64" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="C64" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E64" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F64" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="G64" s="34"/>
-      <c r="H64" s="34"/>
-      <c r="I64" s="33"/>
-      <c r="J64" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K64" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L64" s="33"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:N55" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}"/>
+  <autoFilter ref="A1:N45" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{21527874-0ADF-4209-82A0-BEEB3929A2FA}"/>
@@ -3987,98 +3609,75 @@
     <hyperlink ref="E24" r:id="rId42" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{418DEEFE-D67D-4689-A6E4-8CCA2C059267}"/>
     <hyperlink ref="I24" r:id="rId43" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.106.11.22&amp;effectiveDate=2024-02-05T13:30:06&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{98A2B0FA-9C5E-4835-8C61-1A0CC6C56CDA}"/>
     <hyperlink ref="L24" r:id="rId44" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{AB70A3AA-2A28-4B85-9441-772C138D4B6E}"/>
-    <hyperlink ref="E36" r:id="rId45" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{AA591DB2-7581-46E2-B467-F49155C3C44F}"/>
-    <hyperlink ref="L36" r:id="rId46" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{7A6D0C4C-D2DB-43F9-993C-E3BD7CAD92DD}"/>
-    <hyperlink ref="E37" r:id="rId47" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{0E5CACCC-3BC7-45ED-A665-4B961B6B79FD}"/>
-    <hyperlink ref="H37" r:id="rId48" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=223366009&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{5DB75BFC-D55E-4875-A437-1E620AD1ACE4}"/>
-    <hyperlink ref="L37" r:id="rId49" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0DAFCDC1-3A35-49F9-86A3-EFCE8351E49C}"/>
-    <hyperlink ref="E38" r:id="rId50" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{0F8E1113-3C1F-4098-81AA-D103A3C3E4E1}"/>
-    <hyperlink ref="L38" r:id="rId51" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{889B9854-48EA-4632-81DD-4C6AC8341069}"/>
-    <hyperlink ref="E39" r:id="rId52" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{FD23A05B-2D6F-4CA6-A620-B9D2C5766B78}"/>
-    <hyperlink ref="L39" r:id="rId53" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{926D7745-EF2D-49AD-8F64-AF74702980F3}"/>
-    <hyperlink ref="E40" r:id="rId54" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{463D1E76-10B0-45B7-9680-F5B3B24CC195}"/>
-    <hyperlink ref="L40" r:id="rId55" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.496&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E699B27A-3C84-4DC0-9C6D-C87DFA62EFCD}"/>
-    <hyperlink ref="E42" r:id="rId56" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{21E08D7F-CC64-4EFD-8211-99F5A0A92B3A}"/>
-    <hyperlink ref="L42" r:id="rId57" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.500&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0A4D7A71-024C-4B56-BF9D-06312EDDFF1C}"/>
-    <hyperlink ref="E43" r:id="rId58" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{AD3E600D-6354-4484-B4CE-1CF836CB3054}"/>
-    <hyperlink ref="L43" r:id="rId59" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.501&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{56CCB389-1A8A-4EEA-A783-B92FD345BEA7}"/>
-    <hyperlink ref="E44" r:id="rId60" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{11838974-4C55-46FA-92B4-A485B6B64428}"/>
-    <hyperlink ref="L44" r:id="rId61" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.502&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D871510D-E999-4D2C-99D0-04BF1F5FDF41}"/>
-    <hyperlink ref="E47" r:id="rId62" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{9B4581F7-385E-4379-9BEE-02A167F1905B}"/>
-    <hyperlink ref="L47" r:id="rId63" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{DFCED3FF-24D8-40A9-B08F-9E70FA3370B3}"/>
-    <hyperlink ref="E48" r:id="rId64" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{F7ED96CE-5F04-4A4D-99A2-7537C3B8214B}"/>
-    <hyperlink ref="L48" r:id="rId65" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{315742DA-B29B-4B38-8898-713230484F64}"/>
-    <hyperlink ref="E49" r:id="rId66" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{1DD7FB21-ADBA-43A1-8D64-769C58250348}"/>
-    <hyperlink ref="L49" r:id="rId67" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{81FECE2A-75A0-4F3C-B166-B8CF5C058228}"/>
-    <hyperlink ref="E52" r:id="rId68" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{49D5FF9B-FE40-43A6-A865-3F174F2030FA}"/>
-    <hyperlink ref="L52" r:id="rId69" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4FAB496D-24B1-47A2-A9A0-9552D567398B}"/>
-    <hyperlink ref="E53" r:id="rId70" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7B8E1B66-0D74-498D-8D88-C6351C4F7FB1}"/>
-    <hyperlink ref="L53" r:id="rId71" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E05351A4-8368-4A4B-B12F-961BE504A1A5}"/>
-    <hyperlink ref="E54" r:id="rId72" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{B9A776CF-FC80-4D4E-9655-984F31074E85}"/>
-    <hyperlink ref="L54" r:id="rId73" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A19CC1FA-FBE7-46A2-A89E-FC0E605879FD}"/>
+    <hyperlink ref="E26" r:id="rId45" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{AA591DB2-7581-46E2-B467-F49155C3C44F}"/>
+    <hyperlink ref="L26" r:id="rId46" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{7A6D0C4C-D2DB-43F9-993C-E3BD7CAD92DD}"/>
+    <hyperlink ref="E27" r:id="rId47" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{0E5CACCC-3BC7-45ED-A665-4B961B6B79FD}"/>
+    <hyperlink ref="H27" r:id="rId48" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=223366009&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{5DB75BFC-D55E-4875-A437-1E620AD1ACE4}"/>
+    <hyperlink ref="L27" r:id="rId49" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0DAFCDC1-3A35-49F9-86A3-EFCE8351E49C}"/>
+    <hyperlink ref="E28" r:id="rId50" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{0F8E1113-3C1F-4098-81AA-D103A3C3E4E1}"/>
+    <hyperlink ref="L28" r:id="rId51" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{889B9854-48EA-4632-81DD-4C6AC8341069}"/>
+    <hyperlink ref="E29" r:id="rId52" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{FD23A05B-2D6F-4CA6-A620-B9D2C5766B78}"/>
+    <hyperlink ref="L29" r:id="rId53" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{926D7745-EF2D-49AD-8F64-AF74702980F3}"/>
+    <hyperlink ref="E30" r:id="rId54" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{463D1E76-10B0-45B7-9680-F5B3B24CC195}"/>
+    <hyperlink ref="L30" r:id="rId55" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.496&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E699B27A-3C84-4DC0-9C6D-C87DFA62EFCD}"/>
+    <hyperlink ref="E32" r:id="rId56" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{21E08D7F-CC64-4EFD-8211-99F5A0A92B3A}"/>
+    <hyperlink ref="L32" r:id="rId57" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.500&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0A4D7A71-024C-4B56-BF9D-06312EDDFF1C}"/>
+    <hyperlink ref="E33" r:id="rId58" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{AD3E600D-6354-4484-B4CE-1CF836CB3054}"/>
+    <hyperlink ref="L33" r:id="rId59" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.501&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{56CCB389-1A8A-4EEA-A783-B92FD345BEA7}"/>
+    <hyperlink ref="E34" r:id="rId60" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{11838974-4C55-46FA-92B4-A485B6B64428}"/>
+    <hyperlink ref="L34" r:id="rId61" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.502&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D871510D-E999-4D2C-99D0-04BF1F5FDF41}"/>
+    <hyperlink ref="E37" r:id="rId62" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{9B4581F7-385E-4379-9BEE-02A167F1905B}"/>
+    <hyperlink ref="L37" r:id="rId63" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{DFCED3FF-24D8-40A9-B08F-9E70FA3370B3}"/>
+    <hyperlink ref="E38" r:id="rId64" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{F7ED96CE-5F04-4A4D-99A2-7537C3B8214B}"/>
+    <hyperlink ref="L38" r:id="rId65" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{315742DA-B29B-4B38-8898-713230484F64}"/>
+    <hyperlink ref="E39" r:id="rId66" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{1DD7FB21-ADBA-43A1-8D64-769C58250348}"/>
+    <hyperlink ref="L39" r:id="rId67" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{81FECE2A-75A0-4F3C-B166-B8CF5C058228}"/>
+    <hyperlink ref="E42" r:id="rId68" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{49D5FF9B-FE40-43A6-A865-3F174F2030FA}"/>
+    <hyperlink ref="L42" r:id="rId69" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4FAB496D-24B1-47A2-A9A0-9552D567398B}"/>
+    <hyperlink ref="E43" r:id="rId70" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7B8E1B66-0D74-498D-8D88-C6351C4F7FB1}"/>
+    <hyperlink ref="L43" r:id="rId71" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E05351A4-8368-4A4B-B12F-961BE504A1A5}"/>
+    <hyperlink ref="E44" r:id="rId72" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{B9A776CF-FC80-4D4E-9655-984F31074E85}"/>
+    <hyperlink ref="L44" r:id="rId73" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A19CC1FA-FBE7-46A2-A89E-FC0E605879FD}"/>
     <hyperlink ref="L25" r:id="rId74" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.4&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{6F907670-FA22-4633-9957-BF1722D97459}"/>
     <hyperlink ref="I25" r:id="rId75" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.2.3&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A620A0BE-0D93-418C-8E02-69F661FAE5FD}"/>
     <hyperlink ref="E25" r:id="rId76" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{6429EA44-A0BE-46EC-BF67-7430BB9AAE0F}"/>
-    <hyperlink ref="E46" r:id="rId77" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{210AF206-8EC6-4753-B18F-691F0E018F4B}"/>
-    <hyperlink ref="I46" r:id="rId78" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.5&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A6DE206C-E455-40DC-9E1B-756F49B6FF18}"/>
-    <hyperlink ref="L46" r:id="rId79" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.5&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{15507FCB-F9AC-4DBB-8436-76E49E25C5EF}"/>
-    <hyperlink ref="L45" r:id="rId80" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8E324497-0C3B-4040-AC01-896E177058B3}"/>
-    <hyperlink ref="I45" r:id="rId81" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.6&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CA8E4A7-71BA-4090-8600-26CBB7FEFE64}"/>
-    <hyperlink ref="H45" r:id="rId82" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=394658006&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{721ECB08-9ED5-4D83-9D6F-3E36BCB4E97A}"/>
-    <hyperlink ref="E45" r:id="rId83" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{171680EF-1354-4A0A-B685-C2521C9E7B5B}"/>
+    <hyperlink ref="E36" r:id="rId77" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{210AF206-8EC6-4753-B18F-691F0E018F4B}"/>
+    <hyperlink ref="I36" r:id="rId78" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.5&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A6DE206C-E455-40DC-9E1B-756F49B6FF18}"/>
+    <hyperlink ref="L36" r:id="rId79" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.5&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{15507FCB-F9AC-4DBB-8436-76E49E25C5EF}"/>
+    <hyperlink ref="L35" r:id="rId80" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8E324497-0C3B-4040-AC01-896E177058B3}"/>
+    <hyperlink ref="I35" r:id="rId81" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.6&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CA8E4A7-71BA-4090-8600-26CBB7FEFE64}"/>
+    <hyperlink ref="H35" r:id="rId82" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=394658006&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{721ECB08-9ED5-4D83-9D6F-3E36BCB4E97A}"/>
+    <hyperlink ref="E35" r:id="rId83" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{171680EF-1354-4A0A-B685-C2521C9E7B5B}"/>
     <hyperlink ref="I24" r:id="rId84" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.17.2.4/2020-09-01T00:00:00" xr:uid="{3BC999B2-E1FF-764B-A460-2EFE8CF33320}"/>
     <hyperlink ref="E10" r:id="rId85" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{901B3EB5-29F2-4EB0-906C-663F0E4F00B7}"/>
     <hyperlink ref="L10" r:id="rId86" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.10&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{0BB30E11-298C-4DA7-981F-84CAA9D1E49F}"/>
     <hyperlink ref="H20" r:id="rId87" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{2F46476A-CCBE-47CE-83E8-8C15158702E5}"/>
-    <hyperlink ref="E26" r:id="rId88" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{2EFAD0E2-EF39-4D43-934D-C9B1B5EC46FD}"/>
-    <hyperlink ref="L26" r:id="rId89" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E5CB3AF8-CD35-4336-A52E-F1CD36342B9A}"/>
-    <hyperlink ref="E27" r:id="rId90" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{157CAA35-1F3A-4644-9743-0D3BD7B1AD5D}"/>
-    <hyperlink ref="H27" r:id="rId91" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=223366009&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{B6C54458-5BA4-4CA8-A9E2-5C243DCAF8C7}"/>
-    <hyperlink ref="L27" r:id="rId92" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{400D9654-7241-454F-B4F1-DB0BBFC28C7F}"/>
-    <hyperlink ref="E28" r:id="rId93" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7A911ED1-456E-42DD-8989-6C37E008CB8F}"/>
-    <hyperlink ref="L28" r:id="rId94" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5CD64B4F-E83F-4005-9A6E-787F3DB78C1F}"/>
-    <hyperlink ref="E29" r:id="rId95" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{78F78CB4-BF12-439E-A376-A5EFEAB9638A}"/>
-    <hyperlink ref="L29" r:id="rId96" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.1.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{C9A85D4A-8788-4DF9-97F9-4EB018D4A5B9}"/>
-    <hyperlink ref="E30" r:id="rId97" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{71892660-7F1C-472A-B162-6A37867B13E4}"/>
-    <hyperlink ref="L30" r:id="rId98" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.496&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D5BD9CA3-83A5-49DA-8EDA-EECAF1D8A30A}"/>
-    <hyperlink ref="E32" r:id="rId99" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{A1C783D9-54A1-47F4-8609-B81B79B0BCAC}"/>
-    <hyperlink ref="L32" r:id="rId100" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.500&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{CBF81741-6FE3-47AD-A8C5-5D921B4024A1}"/>
-    <hyperlink ref="E33" r:id="rId101" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{32C938FB-EABD-4ECA-A7CE-58F10B8BE3B9}"/>
-    <hyperlink ref="L33" r:id="rId102" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.501&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{8485E509-F6A8-4CBD-8193-E802481F42A7}"/>
-    <hyperlink ref="E34" r:id="rId103" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{1505873D-5C29-4DF7-8109-CAA50E5FEC45}"/>
-    <hyperlink ref="L34" r:id="rId104" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.121.2.502&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{085BE848-B522-4E53-98CC-F69378ED9E7C}"/>
-    <hyperlink ref="L35" r:id="rId105" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4A02E4C8-6668-4133-8C05-A005AE0BC874}"/>
-    <hyperlink ref="I35" r:id="rId106" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.1.6&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{44E6768D-4906-4177-B6A3-F069389C6FAC}"/>
-    <hyperlink ref="H35" r:id="rId107" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=394658006&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{1EA9AE6D-E4A5-489E-A391-5105421A577E}"/>
-    <hyperlink ref="E35" r:id="rId108" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{412E7912-214B-462C-9DA8-FB6F7B146124}"/>
-    <hyperlink ref="L18" r:id="rId109" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5C01C431-F32A-497B-92D2-4D058995BE9E}"/>
-    <hyperlink ref="I18" r:id="rId110" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.106.11.19&amp;effectiveDate=2024-02-05T12:33:45&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D71DB53F-4DFA-456E-A6FD-A94C4290D1C1}"/>
-    <hyperlink ref="H18" r:id="rId111" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=363698007&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{58172FD2-70FC-4673-BF70-D6AE18467415}"/>
-    <hyperlink ref="E18" r:id="rId112" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{3D0023D3-652A-4840-9808-3B2E5DA099D0}"/>
-    <hyperlink ref="E19" r:id="rId113" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.20.7.2/2020-09-01T00:00:00" xr:uid="{4B3833E8-D6ED-4EC3-8D1E-0F1FF55B206E}"/>
-    <hyperlink ref="E57" r:id="rId114" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{06898B6A-A0ED-0244-9A16-72B56DEBED42}"/>
-    <hyperlink ref="E64" r:id="rId115" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{EABED256-857D-2642-BE3E-5AD20C03336E}"/>
-    <hyperlink ref="E51" r:id="rId116" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{0BB16F56-88D4-5644-B710-8B7860CB1712}"/>
-    <hyperlink ref="I51" r:id="rId117" display="Modalities" xr:uid="{E48A8B75-06B7-5444-866E-89BA6FC9A9FC}"/>
-    <hyperlink ref="E59" r:id="rId118" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{24C31C8F-A2E9-824A-9317-3AA15CB5B012}"/>
-    <hyperlink ref="H59" r:id="rId119" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{C869B80E-2110-5741-BB09-F7EDBF5A7FAE}"/>
-    <hyperlink ref="L59" r:id="rId120" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D915B272-925A-FB46-A898-7CF03503B973}"/>
-    <hyperlink ref="E60" r:id="rId121" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{D7AA8219-AC02-7D4E-9C12-CABC33799EC4}"/>
-    <hyperlink ref="L60" r:id="rId122" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3965CB55-85FB-5D4E-B610-010B1CD32274}"/>
-    <hyperlink ref="E61" r:id="rId123" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{93663DF7-6AD3-2748-912C-FCEE1C2CC562}"/>
-    <hyperlink ref="L61" r:id="rId124" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{F63D6C9B-9ACA-A348-B301-C940CA72AF2C}"/>
-    <hyperlink ref="E62" r:id="rId125" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{F351B801-B480-8645-9B04-58FF53EFC89A}"/>
-    <hyperlink ref="I62" r:id="rId126" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.17.2.4/2020-09-01T00:00:00" xr:uid="{8DDE88C1-182D-284E-AF9A-5977BFBB50BA}"/>
-    <hyperlink ref="L62" r:id="rId127" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{41CE1CBD-75FF-1547-A9BA-108D0AB0450D}"/>
-    <hyperlink ref="L63" r:id="rId128" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.4&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{87455DB6-3D09-9849-9FC5-EBE0AF4C3CEA}"/>
-    <hyperlink ref="I63" r:id="rId129" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.2.3&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{B5CE4245-F76E-3B42-ADA9-69F1DC52B3D6}"/>
-    <hyperlink ref="E63" r:id="rId130" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{7BF95595-025E-BE48-94C3-E19456DD2154}"/>
-    <hyperlink ref="E5" r:id="rId131" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{97B37183-E333-2F40-A93B-078DC30E8909}"/>
-    <hyperlink ref="L5" r:id="rId132" xr:uid="{3C80AA13-A8C0-DB4D-B55B-11C3AC1DD645}"/>
-    <hyperlink ref="E31" r:id="rId133" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{7C87E736-C37B-AD4E-8676-0CEC0731A8C6}"/>
-    <hyperlink ref="L31" r:id="rId134" xr:uid="{AB99BCA2-5B5E-A84E-9445-25F8993321E0}"/>
-    <hyperlink ref="E41" r:id="rId135" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{8E5A2DA5-3A93-9B4F-96B8-A9C383954120}"/>
-    <hyperlink ref="L41" r:id="rId136" xr:uid="{14E761D3-2F17-284C-B1F3-C5DA9DA1930D}"/>
+    <hyperlink ref="L18" r:id="rId88" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{5C01C431-F32A-497B-92D2-4D058995BE9E}"/>
+    <hyperlink ref="I18" r:id="rId89" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.106.11.19&amp;effectiveDate=2024-02-05T12:33:45&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D71DB53F-4DFA-456E-A6FD-A94C4290D1C1}"/>
+    <hyperlink ref="H18" r:id="rId90" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=363698007&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{58172FD2-70FC-4673-BF70-D6AE18467415}"/>
+    <hyperlink ref="E18" r:id="rId91" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{3D0023D3-652A-4840-9808-3B2E5DA099D0}"/>
+    <hyperlink ref="E19" r:id="rId92" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.20.7.2/2020-09-01T00:00:00" xr:uid="{4B3833E8-D6ED-4EC3-8D1E-0F1FF55B206E}"/>
+    <hyperlink ref="E47" r:id="rId93" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{06898B6A-A0ED-0244-9A16-72B56DEBED42}"/>
+    <hyperlink ref="E54" r:id="rId94" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{EABED256-857D-2642-BE3E-5AD20C03336E}"/>
+    <hyperlink ref="E41" r:id="rId95" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{0BB16F56-88D4-5644-B710-8B7860CB1712}"/>
+    <hyperlink ref="I41" r:id="rId96" display="Modalities" xr:uid="{E48A8B75-06B7-5444-866E-89BA6FC9A9FC}"/>
+    <hyperlink ref="E49" r:id="rId97" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{24C31C8F-A2E9-824A-9317-3AA15CB5B012}"/>
+    <hyperlink ref="H49" r:id="rId98" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=257622000&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{C869B80E-2110-5741-BB09-F7EDBF5A7FAE}"/>
+    <hyperlink ref="L49" r:id="rId99" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{D915B272-925A-FB46-A898-7CF03503B973}"/>
+    <hyperlink ref="E50" r:id="rId100" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{D7AA8219-AC02-7D4E-9C12-CABC33799EC4}"/>
+    <hyperlink ref="L50" r:id="rId101" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3965CB55-85FB-5D4E-B610-010B1CD32274}"/>
+    <hyperlink ref="E51" r:id="rId102" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{93663DF7-6AD3-2748-912C-FCEE1C2CC562}"/>
+    <hyperlink ref="L51" r:id="rId103" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.3&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{F63D6C9B-9ACA-A348-B301-C940CA72AF2C}"/>
+    <hyperlink ref="E52" r:id="rId104" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{F351B801-B480-8645-9B04-58FF53EFC89A}"/>
+    <hyperlink ref="I52" r:id="rId105" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.17.2.4/2020-09-01T00:00:00" xr:uid="{8DDE88C1-182D-284E-AF9A-5977BFBB50BA}"/>
+    <hyperlink ref="L52" r:id="rId106" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{41CE1CBD-75FF-1547-A9BA-108D0AB0450D}"/>
+    <hyperlink ref="L53" r:id="rId107" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.4&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{87455DB6-3D09-9849-9FC5-EBE0AF4C3CEA}"/>
+    <hyperlink ref="I53" r:id="rId108" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.2.3&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{B5CE4245-F76E-3B42-ADA9-69F1DC52B3D6}"/>
+    <hyperlink ref="E53" r:id="rId109" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{7BF95595-025E-BE48-94C3-E19456DD2154}"/>
+    <hyperlink ref="E5" r:id="rId110" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{97B37183-E333-2F40-A93B-078DC30E8909}"/>
+    <hyperlink ref="L5" r:id="rId111" xr:uid="{3C80AA13-A8C0-DB4D-B55B-11C3AC1DD645}"/>
+    <hyperlink ref="E31" r:id="rId112" location="String" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - String" xr:uid="{8E5A2DA5-3A93-9B4F-96B8-A9C383954120}"/>
+    <hyperlink ref="L31" r:id="rId113" xr:uid="{14E761D3-2F17-284C-B1F3-C5DA9DA1930D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4121,7 +3720,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -4171,10 +3770,10 @@
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>14</v>
@@ -4186,23 +3785,23 @@
         <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="H3" s="28"/>
       <c r="J3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
@@ -4214,14 +3813,14 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="H4" s="27"/>
       <c r="J4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="L4" s="3"/>
     </row>
@@ -4295,7 +3894,7 @@
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>23</v>
@@ -4375,10 +3974,10 @@
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>14</v>
@@ -4390,7 +3989,7 @@
         <v>34</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
@@ -4402,12 +4001,12 @@
         <v>36</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>38</v>
@@ -4434,7 +4033,7 @@
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>41</v>
@@ -4449,7 +4048,7 @@
         <v>34</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>19</v>
@@ -4463,7 +4062,7 @@
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>45</v>
@@ -4539,7 +4138,7 @@
         <v>53</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>19</v>
@@ -4568,7 +4167,7 @@
         <v>58</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>60</v>
@@ -4611,20 +4210,20 @@
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="19" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -4639,10 +4238,10 @@
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>14</v>
@@ -4654,7 +4253,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -4663,16 +4262,16 @@
         <v>19</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="L14" s="21"/>
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>14</v>
@@ -4684,7 +4283,7 @@
         <v>53</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -4693,34 +4292,34 @@
         <v>19</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="L15" s="21"/>
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="4"/>
@@ -4729,20 +4328,20 @@
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="38" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -4753,20 +4352,20 @@
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="19" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -4781,10 +4380,10 @@
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>14</v>
@@ -4796,7 +4395,7 @@
         <v>16</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -4805,16 +4404,16 @@
         <v>19</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="L19" s="21"/>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>14</v>
@@ -4826,7 +4425,7 @@
         <v>53</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -4835,34 +4434,34 @@
         <v>19</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="L20" s="21"/>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
@@ -4871,10 +4470,10 @@
     </row>
     <row r="22" spans="1:14" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>14</v>
@@ -4884,17 +4483,17 @@
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="38" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4946,12 +4545,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5184,20 +4785,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5222,12 +4824,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DOSINZAGE2-740: Changed cardinality of ReportTitle/ImageTitle
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E59351-303B-654C-9872-AFDE7F20F298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4246830-322D-214E-9896-317A13BED8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="660" windowWidth="38080" windowHeight="19380" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="264">
   <si>
     <t>Naam</t>
   </si>
@@ -537,9 +537,6 @@
   </si>
   <si>
     <t>bbs-medmij-dataelement-1</t>
-  </si>
-  <si>
-    <t>1…1</t>
   </si>
   <si>
     <t>Titel van het verslag</t>
@@ -1401,10 +1398,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1824,7 +1821,7 @@
       <c r="D2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="70" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="66" t="s">
@@ -1833,15 +1830,15 @@
       <c r="G2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
       <c r="J2" s="66" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="68" t="s">
+      <c r="L2" s="70" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1850,17 +1847,22 @@
       <c r="B3" s="67"/>
       <c r="C3" s="67"/>
       <c r="D3" s="67"/>
-      <c r="E3" s="69"/>
+      <c r="E3" s="71"/>
       <c r="F3" s="67"/>
       <c r="G3" s="67"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
       <c r="J3" s="67"/>
       <c r="K3" s="67"/>
-      <c r="L3" s="69"/>
+      <c r="L3" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1868,11 +1870,6 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1886,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2028,10 +2025,10 @@
     </row>
     <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>249</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>250</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>14</v>
@@ -2043,7 +2040,7 @@
         <v>34</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
@@ -2055,12 +2052,12 @@
         <v>36</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>38</v>
@@ -2090,7 +2087,7 @@
     </row>
     <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>41</v>
@@ -2122,7 +2119,7 @@
     </row>
     <row r="8" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>45</v>
@@ -2385,7 +2382,7 @@
         <v>58</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
@@ -2418,7 +2415,7 @@
       </c>
       <c r="E17" s="33"/>
       <c r="F17" s="61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G17" s="34"/>
       <c r="H17" s="33" t="s">
@@ -2483,7 +2480,7 @@
         <v>58</v>
       </c>
       <c r="F19" s="60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J19" s="32" t="s">
         <v>19</v>
@@ -2494,7 +2491,7 @@
     </row>
     <row r="20" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>94</v>
@@ -2524,7 +2521,7 @@
     </row>
     <row r="21" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="51" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>97</v>
@@ -2682,7 +2679,7 @@
     </row>
     <row r="26" spans="1:12" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B26" s="32" t="s">
         <v>139</v>
@@ -2691,11 +2688,11 @@
         <v>14</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E26" s="33"/>
       <c r="F26" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J26" s="32" t="s">
         <v>25</v>
@@ -2767,7 +2764,7 @@
     </row>
     <row r="29" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>143</v>
@@ -2829,10 +2826,10 @@
     </row>
     <row r="31" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="B31" s="32" t="s">
         <v>256</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>257</v>
       </c>
       <c r="C31" s="32" t="s">
         <v>14</v>
@@ -2844,7 +2841,7 @@
         <v>34</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
@@ -2856,12 +2853,12 @@
         <v>36</v>
       </c>
       <c r="L31" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B32" s="32" t="s">
         <v>145</v>
@@ -2891,7 +2888,7 @@
     </row>
     <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="42" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B33" s="32" t="s">
         <v>146</v>
@@ -2923,7 +2920,7 @@
     </row>
     <row r="34" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>147</v>
@@ -2989,7 +2986,7 @@
     </row>
     <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B36" s="32" t="s">
         <v>149</v>
@@ -3036,7 +3033,7 @@
       </c>
       <c r="E37" s="33"/>
       <c r="F37" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G37" s="34"/>
       <c r="H37" s="34"/>
@@ -3066,7 +3063,7 @@
         <v>16</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G38" s="34"/>
       <c r="H38" s="34"/>
@@ -3120,13 +3117,13 @@
         <v>14</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F40" s="60" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I40" s="12"/>
       <c r="J40" s="11" t="s">
@@ -3139,27 +3136,27 @@
     </row>
     <row r="41" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="B41" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="B41" s="32" t="s">
-        <v>212</v>
-      </c>
       <c r="C41" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E41" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J41" s="32" t="s">
         <v>19</v>
@@ -3169,15 +3166,15 @@
       </c>
       <c r="L41" s="33"/>
       <c r="M41" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" s="32" t="s">
         <v>168</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>169</v>
       </c>
       <c r="C42" s="32" t="s">
         <v>14</v>
@@ -3187,7 +3184,7 @@
       </c>
       <c r="E42" s="33"/>
       <c r="F42" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
@@ -3202,10 +3199,10 @@
     </row>
     <row r="43" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="32" t="s">
         <v>170</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>171</v>
       </c>
       <c r="C43" s="32" t="s">
         <v>14</v>
@@ -3217,7 +3214,7 @@
         <v>16</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
@@ -3226,16 +3223,16 @@
         <v>19</v>
       </c>
       <c r="K43" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L43" s="33"/>
     </row>
     <row r="44" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" s="32" t="s">
         <v>173</v>
-      </c>
-      <c r="B44" s="32" t="s">
-        <v>174</v>
       </c>
       <c r="C44" s="32" t="s">
         <v>14</v>
@@ -3247,7 +3244,7 @@
         <v>53</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="34"/>
@@ -3256,53 +3253,53 @@
         <v>19</v>
       </c>
       <c r="K44" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L44" s="33"/>
     </row>
     <row r="45" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>177</v>
-      </c>
       <c r="C45" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F45" s="60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I45" s="12"/>
       <c r="J45" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L45" s="12"/>
     </row>
     <row r="46" spans="1:13" s="50" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C46" s="50" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="F46" s="62" t="s">
         <v>229</v>
-      </c>
-      <c r="F46" s="62" t="s">
-        <v>230</v>
       </c>
       <c r="G46" s="57"/>
       <c r="H46" s="57"/>
@@ -3317,22 +3314,22 @@
     </row>
     <row r="47" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C47" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E47" s="33" t="s">
         <v>16</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G47" s="34"/>
       <c r="H47" s="34"/>
@@ -3341,26 +3338,26 @@
         <v>19</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L47" s="33"/>
     </row>
     <row r="48" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C48" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E48" s="33"/>
       <c r="F48" s="30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
@@ -3369,22 +3366,22 @@
         <v>19</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L48" s="33"/>
     </row>
     <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C49" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E49" s="33"/>
       <c r="F49" s="30" t="s">
@@ -3405,16 +3402,16 @@
     </row>
     <row r="50" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C50" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E50" s="33" t="s">
         <v>16</v>
@@ -3437,10 +3434,10 @@
     </row>
     <row r="51" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C51" s="32" t="s">
         <v>14</v>
@@ -3472,7 +3469,7 @@
         <v>109</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C52" s="32" t="s">
         <v>14</v>
@@ -3501,10 +3498,10 @@
     </row>
     <row r="53" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>14</v>
@@ -3533,10 +3530,10 @@
     </row>
     <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C54" s="32" t="s">
         <v>14</v>
@@ -3548,7 +3545,7 @@
         <v>16</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G54" s="34"/>
       <c r="H54" s="34"/>
@@ -3720,7 +3717,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -3770,7 +3767,7 @@
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>157</v>
@@ -3798,7 +3795,7 @@
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>157</v>
@@ -3842,7 +3839,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3894,7 +3891,7 @@
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>23</v>
@@ -3974,10 +3971,10 @@
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>249</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>250</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>14</v>
@@ -3989,7 +3986,7 @@
         <v>34</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
@@ -4001,12 +3998,12 @@
         <v>36</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>38</v>
@@ -4033,7 +4030,7 @@
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>41</v>
@@ -4048,7 +4045,7 @@
         <v>34</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>19</v>
@@ -4062,7 +4059,7 @@
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>45</v>
@@ -4138,7 +4135,7 @@
         <v>53</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>19</v>
@@ -4167,7 +4164,7 @@
         <v>58</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>60</v>
@@ -4210,20 +4207,20 @@
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>155</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -4238,7 +4235,7 @@
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>157</v>
@@ -4253,7 +4250,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -4268,7 +4265,7 @@
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>161</v>
@@ -4298,7 +4295,7 @@
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>164</v>
@@ -4307,19 +4304,19 @@
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="4"/>
@@ -4328,20 +4325,20 @@
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="C17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -4352,20 +4349,20 @@
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>155</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -4380,10 +4377,10 @@
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>14</v>
@@ -4395,7 +4392,7 @@
         <v>16</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -4410,10 +4407,10 @@
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>14</v>
@@ -4425,7 +4422,7 @@
         <v>53</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -4440,28 +4437,28 @@
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
@@ -4470,10 +4467,10 @@
     </row>
     <row r="22" spans="1:14" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>14</v>
@@ -4483,17 +4480,17 @@
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -4545,17 +4542,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100597771DCE5E0DD409E6796B5544574D3" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1f155c61874143f60c84865cea76726f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xmlns:ns3="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7515b2bcca035c7557d524d6ba7a724c" ns2:_="" ns3:_="">
     <xsd:import namespace="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
@@ -4784,6 +4770,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4794,17 +4791,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{815FF2A9-0500-4E41-8F16-110FB0128C02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4823,6 +4809,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
   <ds:schemaRefs>

</xml_diff>